<commit_message>
export spreadsheet that includes missing entries
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -2650,12 +2650,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
     </row>
@@ -2665,12 +2665,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2680,12 +2680,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
         </is>
       </c>
     </row>
@@ -2695,12 +2695,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -2710,12 +2710,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t xml:space="preserve">P8213 </t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:t-vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -2725,12 +2725,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">P8205 </t>
+          <t xml:space="preserve">P4CZ16780 </t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:band-yesh-d-'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -2740,12 +2740,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">P8222 </t>
+          <t xml:space="preserve">P1KG8854 </t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:jnanasidhi'}</t>
+          <t>{'eft:srilendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -2755,12 +2755,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -2770,12 +2770,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -2785,12 +2785,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -2800,12 +2800,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -2815,12 +2815,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -2830,12 +2830,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -2845,12 +2845,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -2860,12 +2860,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -2875,12 +2875,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve">P3285 </t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -2890,12 +2890,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
     </row>
@@ -2905,12 +2905,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
     </row>
@@ -2920,12 +2920,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -2935,12 +2935,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -2950,12 +2950,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -2965,12 +2965,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve">P3214 </t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2980,12 +2980,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -2995,12 +2995,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -3010,12 +3010,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:yesh-nyingpo', 'eft:ye-shes-snying-po', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:jnanasiddhi'}</t>
         </is>
       </c>
     </row>
@@ -3025,12 +3025,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -3040,12 +3040,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t xml:space="preserve">P8205 </t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:band-yesh-d-'}</t>
         </is>
       </c>
     </row>
@@ -3055,12 +3055,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -3070,12 +3070,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t xml:space="preserve">P3285 </t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -3085,12 +3085,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -3100,12 +3100,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3115,12 +3115,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t xml:space="preserve">P4CZ16780 </t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -3130,12 +3130,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
     </row>
@@ -3145,12 +3145,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t xml:space="preserve">P3214 </t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3160,12 +3160,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -3175,12 +3175,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -3190,12 +3190,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t xml:space="preserve">P1KG8854 </t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:srilendrabodhi'}</t>
+          <t>{'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po'}</t>
         </is>
       </c>
     </row>
@@ -3205,12 +3205,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
     </row>
@@ -3220,12 +3220,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -3235,12 +3235,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3250,12 +3250,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3265,12 +3265,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t xml:space="preserve">P3709 </t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -3280,12 +3280,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3295,12 +3295,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -3310,12 +3310,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -3325,12 +3325,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -3340,12 +3340,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
     </row>
@@ -3355,12 +3355,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P8210</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
     </row>
@@ -3370,12 +3370,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t xml:space="preserve">P3709 </t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3385,12 +3385,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
     </row>
@@ -3400,12 +3400,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t xml:space="preserve">P8222 </t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:jnanasidhi'}</t>
         </is>
       </c>
     </row>
@@ -3415,12 +3415,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -3430,12 +3430,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -3445,12 +3445,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -3460,12 +3460,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t xml:space="preserve">P8213 </t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>{'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3475,12 +3475,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:yesh-nyingpo', 'eft:ye-shes-snying-po', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3490,12 +3490,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8210</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3505,12 +3505,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -3520,12 +3520,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
iterate through matching attributions from spreadsheet
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -2650,12 +2650,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -2665,12 +2665,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -2680,12 +2680,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -2695,12 +2695,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t xml:space="preserve">P3285 </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -2710,12 +2710,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t xml:space="preserve">P8222 </t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:jnanasidhi'}</t>
         </is>
       </c>
     </row>
@@ -2725,12 +2725,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -2740,12 +2740,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">P8205 </t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:band-yesh-d-'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -2755,12 +2755,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -2770,12 +2770,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -2785,12 +2785,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">P8222 </t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:jnanasidhi'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2800,12 +2800,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -2815,12 +2815,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -2830,12 +2830,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
     </row>
@@ -2845,12 +2845,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P8210</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2860,12 +2860,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t xml:space="preserve">P8205 </t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:band-yesh-d-'}</t>
         </is>
       </c>
     </row>
@@ -2875,12 +2875,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
     </row>
@@ -2890,12 +2890,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -2905,12 +2905,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve">P3214 </t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs'}</t>
         </is>
       </c>
     </row>
@@ -2920,12 +2920,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -2935,12 +2935,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -2950,12 +2950,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">P1KG8854 </t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:srilendrabodhi'}</t>
+          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de'}</t>
         </is>
       </c>
     </row>
@@ -2965,12 +2965,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -2980,12 +2980,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -2995,12 +2995,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
     </row>
@@ -3010,12 +3010,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -3025,12 +3025,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3040,12 +3040,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -3055,12 +3055,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -3070,12 +3070,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -3085,12 +3085,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
     </row>
@@ -3100,12 +3100,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -3115,12 +3115,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -3130,12 +3130,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P8210</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3145,12 +3145,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t xml:space="preserve">P8213 </t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:t-vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -3160,12 +3160,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3175,12 +3175,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:jnanasiddhi'}</t>
         </is>
       </c>
     </row>
@@ -3190,12 +3190,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t xml:space="preserve">P8213 </t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -3205,12 +3205,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t xml:space="preserve">P3709 </t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -3220,12 +3220,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:yesh-nyingpo', 'eft:t-jnanagarbha', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
     </row>
@@ -3235,12 +3235,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3250,12 +3250,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -3265,12 +3265,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t xml:space="preserve">P4CZ16780 </t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
         </is>
       </c>
     </row>
@@ -3280,12 +3280,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -3295,12 +3295,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3310,12 +3310,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t xml:space="preserve">P4CZ16780 </t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -3325,12 +3325,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -3340,12 +3340,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -3355,12 +3355,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t xml:space="preserve">P1KG8854 </t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:srilendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3370,12 +3370,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3385,12 +3385,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t xml:space="preserve">P3709 </t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -3400,12 +3400,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs'}</t>
+          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
         </is>
       </c>
     </row>
@@ -3415,12 +3415,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t xml:space="preserve">P3214 </t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3430,12 +3430,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:ye-shes-snying-po', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
     </row>
@@ -3445,12 +3445,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -3460,12 +3460,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3475,12 +3475,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
     </row>
@@ -3490,12 +3490,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -3505,12 +3505,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t xml:space="preserve">P3285 </t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3520,12 +3520,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add 84000 ids to new_attributions file, rename column that wasn't parsing
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -2650,12 +2650,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t xml:space="preserve">P4CZ16780 </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -2665,12 +2665,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t xml:space="preserve">P8213 </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
+          <t>{'eft:t-vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -2680,12 +2680,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -2695,12 +2695,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -2710,12 +2710,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2725,12 +2725,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
     </row>
@@ -2740,12 +2740,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:yesh-d-', 'eft:band-yesh-de', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
     </row>
@@ -2755,12 +2755,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -2770,12 +2770,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
     </row>
@@ -2785,12 +2785,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
     </row>
@@ -2800,12 +2800,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t xml:space="preserve">P3285 </t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -2815,12 +2815,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -2830,12 +2830,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -2845,12 +2845,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -2860,12 +2860,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -2875,12 +2875,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -2890,12 +2890,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P8210</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -2905,12 +2905,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t xml:space="preserve">P3709 </t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -2920,12 +2920,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -2935,12 +2935,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:ye-shes-snying-po', 'eft:yesh-nyingpo', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -2950,12 +2950,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -2965,12 +2965,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve">P3214 </t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:jnanasiddhi'}</t>
         </is>
       </c>
     </row>
@@ -2980,12 +2980,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P8210</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -2995,12 +2995,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -3010,12 +3010,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t xml:space="preserve">P8222 </t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:jnanasidhi'}</t>
         </is>
       </c>
     </row>
@@ -3025,12 +3025,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve">P8222 </t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:jnanasidhi'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3040,12 +3040,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t xml:space="preserve">P8205 </t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:band-yesh-d-'}</t>
         </is>
       </c>
     </row>
@@ -3055,12 +3055,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t xml:space="preserve">P3214 </t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3070,12 +3070,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -3085,12 +3085,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -3100,12 +3100,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -3115,12 +3115,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t xml:space="preserve">P1KG8854 </t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:srilendrabodhi'}</t>
+          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
         </is>
       </c>
     </row>
@@ -3130,12 +3130,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
     </row>
@@ -3145,12 +3145,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -3160,12 +3160,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -3175,12 +3175,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t xml:space="preserve">P3285 </t>
+          <t>?</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -3190,12 +3190,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -3205,12 +3205,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3220,12 +3220,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t xml:space="preserve">P3709 </t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -3235,12 +3235,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3250,12 +3250,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -3265,12 +3265,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -3280,12 +3280,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t xml:space="preserve">P8205 </t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:band-yesh-d-'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -3295,12 +3295,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t xml:space="preserve">P8213 </t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3310,12 +3310,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
         </is>
       </c>
     </row>
@@ -3325,12 +3325,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t xml:space="preserve">P4CZ16780 </t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -3340,12 +3340,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -3355,12 +3355,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3370,12 +3370,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3385,12 +3385,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -3400,12 +3400,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -3415,12 +3415,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:paltsek', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs'}</t>
         </is>
       </c>
     </row>
@@ -3430,12 +3430,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3445,12 +3445,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -3460,12 +3460,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t xml:space="preserve">P1KG8854 </t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:srilendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3475,12 +3475,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -3490,12 +3490,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
     </row>
@@ -3505,12 +3505,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
     </row>
@@ -3520,12 +3520,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix manual data, add resource to new attribution entries
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -1642,7 +1642,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t xml:space="preserve">P3214 </t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="D56" t="inlineStr"/>
@@ -1672,7 +1672,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t xml:space="preserve">P8213 </t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="D57" t="inlineStr"/>
@@ -1732,7 +1732,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t xml:space="preserve">P8205 </t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="D59" t="inlineStr"/>
@@ -1852,7 +1852,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t xml:space="preserve">P1KG8854 </t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="D63" t="inlineStr"/>
@@ -2144,7 +2144,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t xml:space="preserve">P8222 </t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="D73" t="inlineStr"/>
@@ -2234,7 +2234,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t xml:space="preserve">P4CZ16780 </t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="D76" t="inlineStr"/>
@@ -2354,7 +2354,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t xml:space="preserve">P3285 </t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="D80" t="inlineStr"/>
@@ -2444,7 +2444,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t xml:space="preserve">P3709 </t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="D83" t="inlineStr"/>
@@ -2624,7 +2624,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2650,12 +2650,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">P4CZ16780 </t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2665,12 +2665,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">P8213 </t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -2680,12 +2680,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -2695,12 +2695,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po'}</t>
         </is>
       </c>
     </row>
@@ -2710,12 +2710,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
         </is>
       </c>
     </row>
@@ -2725,12 +2725,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -2740,12 +2740,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:yesh-d-', 'eft:band-yesh-de', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
     </row>
@@ -2755,12 +2755,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -2785,12 +2785,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
     </row>
@@ -2800,12 +2800,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve">P3285 </t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -2815,12 +2815,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -2830,12 +2830,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2845,12 +2845,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -2860,12 +2860,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -2875,12 +2875,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -2905,12 +2905,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve">P3709 </t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
         </is>
       </c>
     </row>
@@ -2920,12 +2920,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
     </row>
@@ -2935,12 +2935,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:yesh-nyingpo', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -2950,12 +2950,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -2965,12 +2965,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -2980,12 +2980,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -2995,12 +2995,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -3010,12 +3010,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve">P8222 </t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:jnanasidhi'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
     </row>
@@ -3025,12 +3025,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -3040,12 +3040,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve">P8205 </t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:band-yesh-d-'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3055,12 +3055,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve">P3214 </t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3070,12 +3070,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
     </row>
@@ -3085,12 +3085,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -3100,12 +3100,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
     </row>
@@ -3115,12 +3115,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:srilendrabodhi', 'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3130,12 +3130,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -3145,12 +3145,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
         </is>
       </c>
     </row>
@@ -3160,12 +3160,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -3175,12 +3175,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -3190,12 +3190,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -3205,12 +3205,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -3220,12 +3220,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -3235,12 +3235,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -3250,12 +3250,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3265,12 +3265,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3280,12 +3280,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -3295,12 +3295,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -3310,12 +3310,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -3325,12 +3325,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -3340,12 +3340,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3355,12 +3355,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -3370,12 +3370,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -3385,12 +3385,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde', 'eft:band-yesh-d-', 'eft:yesh-d-'}</t>
         </is>
       </c>
     </row>
@@ -3400,12 +3400,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -3415,12 +3415,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:paltsek', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -3430,12 +3430,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -3445,12 +3445,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -3460,72 +3460,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t xml:space="preserve">P1KG8854 </t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>{'eft:srilendrabodhi'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>P2637</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>P3379</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>P8266</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>P3456</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
remove unknown from URI
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -2650,12 +2650,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -2665,12 +2665,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -2680,12 +2680,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -2695,12 +2695,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2710,12 +2710,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -2725,12 +2725,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -2740,12 +2740,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
+          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
         </is>
       </c>
     </row>
@@ -2755,12 +2755,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
         </is>
       </c>
     </row>
@@ -2770,12 +2770,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po'}</t>
         </is>
       </c>
     </row>
@@ -2785,12 +2785,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
     </row>
@@ -2800,12 +2800,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -2815,12 +2815,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -2830,12 +2830,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
     </row>
@@ -2845,12 +2845,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:yesh-d-'}</t>
         </is>
       </c>
     </row>
@@ -2860,12 +2860,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
     </row>
@@ -2875,12 +2875,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
     </row>
@@ -2890,12 +2890,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P8210</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
     </row>
@@ -2905,12 +2905,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -2920,12 +2920,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -2935,12 +2935,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:srilendrabodhi', 'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -2950,12 +2950,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -2965,12 +2965,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -2980,12 +2980,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
         </is>
       </c>
     </row>
@@ -3010,12 +3010,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -3025,12 +3025,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P8210</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3040,12 +3040,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -3055,12 +3055,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -3070,12 +3070,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
         </is>
       </c>
     </row>
@@ -3085,12 +3085,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -3100,12 +3100,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -3115,12 +3115,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:srilendrabodhi', 'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3130,12 +3130,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3145,12 +3145,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -3160,12 +3160,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
     </row>
@@ -3175,12 +3175,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -3190,12 +3190,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -3205,12 +3205,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -3220,12 +3220,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -3235,12 +3235,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -3250,12 +3250,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -3265,12 +3265,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3280,12 +3280,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3295,12 +3295,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -3310,12 +3310,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -3325,12 +3325,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3340,12 +3340,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -3355,12 +3355,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -3370,12 +3370,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3385,12 +3385,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:ye-shes-sde', 'eft:band-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3400,12 +3400,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -3415,12 +3415,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -3430,12 +3430,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3445,12 +3445,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3460,12 +3460,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update spreadsheet with language attribution
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -2650,12 +2650,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -2665,12 +2665,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
         </is>
       </c>
     </row>
@@ -2680,12 +2680,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -2695,12 +2695,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
     </row>
@@ -2710,12 +2710,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -2725,12 +2725,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2740,12 +2740,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -2755,12 +2755,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -2770,12 +2770,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po'}</t>
+          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
         </is>
       </c>
     </row>
@@ -2785,12 +2785,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -2800,12 +2800,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -2815,12 +2815,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -2830,12 +2830,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -2845,12 +2845,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:yesh-d-'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -2860,12 +2860,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -2875,12 +2875,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -2890,12 +2890,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
     </row>
@@ -2905,12 +2905,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -2920,12 +2920,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:band-yesh-d-'}</t>
         </is>
       </c>
     </row>
@@ -2935,12 +2935,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:srilendrabodhi', 'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -2950,12 +2950,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -2965,12 +2965,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -2980,12 +2980,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -2995,12 +2995,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
         </is>
       </c>
     </row>
@@ -3010,12 +3010,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
     </row>
@@ -3025,12 +3025,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P8210</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -3055,12 +3055,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3070,12 +3070,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -3085,12 +3085,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3100,12 +3100,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3115,12 +3115,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3130,12 +3130,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -3145,12 +3145,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -3160,12 +3160,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -3175,12 +3175,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3190,12 +3190,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -3205,12 +3205,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -3220,12 +3220,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -3235,12 +3235,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
     </row>
@@ -3250,12 +3250,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -3265,12 +3265,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3280,12 +3280,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
     </row>
@@ -3295,12 +3295,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -3310,12 +3310,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -3325,12 +3325,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -3340,12 +3340,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
     </row>
@@ -3355,12 +3355,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -3370,12 +3370,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P8210</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3385,12 +3385,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
     </row>
@@ -3400,12 +3400,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -3415,12 +3415,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3430,12 +3430,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
     </row>
@@ -3445,12 +3445,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -3460,12 +3460,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
get attributions for hyphenated works
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H88"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,12 +477,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>eft:jinamitra-k-</t>
+          <t>eft:sarvajnadeva</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -497,12 +497,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>eft:klu-i-rgyal-mtshan</t>
+          <t>eft:vidyakaraprabha</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -517,12 +517,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>eft:dzi-na-mi-tra-k-</t>
+          <t>eft:dharmakara</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -537,12 +537,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>eft:cog-ro-klu-i-rgyal-mtshan</t>
+          <t>eft:jinamitra-k-</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -557,12 +557,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>eft:dharmakara</t>
+          <t>eft:klu-i-rgyal-mtshan</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -577,12 +577,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>eft:ban-de-dpal-gyi-lhun-po</t>
+          <t>eft:dzi-na-mi-tra-k-</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -597,12 +597,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>eft:ban-de-dpal-brtsegs</t>
+          <t>eft:cog-ro-klu-i-rgyal-mtshan</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -617,12 +617,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>eft:dpal-byor</t>
+          <t>eft:ban-de-dpal-gyi-lhun-po</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -637,12 +637,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>eft:surendrabodhi</t>
+          <t>eft:ban-de-dpal-brtsegs</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -657,12 +657,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>eft:jinamitra</t>
+          <t>eft:dpal-byor</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -677,12 +677,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>eft:danasila</t>
+          <t>eft:surendrabodhi</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>P8210</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -697,12 +697,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>eft:prajnavarman</t>
+          <t>eft:jinamitra</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -717,12 +717,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>eft:dpal-dbyangs</t>
+          <t>eft:danasila</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P8210</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -737,12 +737,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>eft:ska-ba-dpal-brtsegs</t>
+          <t>eft:prajnavarman</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -757,12 +757,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>eft:munivarman</t>
+          <t>eft:dpal-dbyangs</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -777,12 +777,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>eft:silendrabodhi</t>
+          <t>eft:ska-ba-dpal-brtsegs</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
@@ -797,12 +797,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>eft:prajnavarma</t>
+          <t>eft:munivarman</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
@@ -817,12 +817,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>eft:buddhaprabha</t>
+          <t>eft:silendrabodhi</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
@@ -837,12 +837,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>eft:ye-shes-sde</t>
+          <t>eft:prajnavarma</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
@@ -857,12 +857,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>eft:dgon-gling-rma</t>
+          <t>eft:buddhaprabha</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
@@ -877,12 +877,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>eft:dpal-gyi-lhun-po</t>
+          <t>eft:ye-shes-sde</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
@@ -897,12 +897,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>eft:dpal-brtsegs</t>
+          <t>eft:dgon-gling-rma</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
@@ -917,12 +917,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>eft:sakyaprabha</t>
+          <t>eft:dpal-gyi-lhun-po</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
@@ -937,12 +937,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>eft:dharmatasila</t>
+          <t>eft:dpal-brtsegs</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
@@ -957,12 +957,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>eft:ye-shes-snying-po</t>
+          <t>eft:sakyaprabha</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
@@ -977,12 +977,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>eft:visuddhasimha</t>
+          <t>eft:dharmatasila</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
@@ -997,12 +997,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>eft:dge-ba-dpal</t>
+          <t>eft:ye-shes-snying-po</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
@@ -1017,12 +1017,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>eft:devacandra</t>
+          <t>eft:visuddhasimha</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
@@ -1037,12 +1037,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>eft:kamalagupta</t>
+          <t>eft:dge-ba-dpal</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
@@ -1057,12 +1057,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>eft:rin-chen-bzang-po</t>
+          <t>eft:devacandra</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
@@ -1077,12 +1077,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>eft:rin-chen-tsho</t>
+          <t>eft:kamalagupta</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
@@ -1097,12 +1097,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>eft:jnanagarbha</t>
+          <t>eft:rin-chen-bzang-po</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
@@ -1117,12 +1117,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>eft:sarvajnadeva</t>
+          <t>eft:rin-chen-tsho</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
@@ -1137,12 +1137,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>eft:vijayasila</t>
+          <t>eft:jnanagarbha</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
@@ -1157,12 +1157,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>eft:hwa-shang-zab-mo</t>
+          <t>eft:vijayasila</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
@@ -1177,12 +1177,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>eft:rnam-par-mi-rtog-pa</t>
+          <t>eft:hwa-shang-zab-mo</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
@@ -1197,12 +1197,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>eft:munivarma</t>
+          <t>eft:rnam-par-mi-rtog-pa</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="D38" t="inlineStr"/>
@@ -1217,12 +1217,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>eft:ratnaraksita</t>
+          <t>eft:munivarma</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
@@ -1237,12 +1237,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>eft:dharmasribhadra</t>
+          <t>eft:ratnaraksita</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
@@ -1257,12 +1257,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>eft:gayadhara</t>
+          <t>eft:dharmasribhadra</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
@@ -1277,12 +1277,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>eft:krsnapandita</t>
+          <t>eft:gayadhara</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
@@ -1297,12 +1297,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>eft:tshul-khrims-rgyal-ba</t>
+          <t>eft:krsnapandita</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
@@ -1317,12 +1317,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>eft:celu</t>
+          <t>eft:tshul-khrims-rgyal-ba</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
@@ -1337,12 +1337,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>eft:jnanasiddhi</t>
+          <t>eft:celu</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="D45" t="inlineStr"/>
@@ -1357,12 +1357,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>eft:punyasambhava</t>
+          <t>eft:jnanasiddhi</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="D46" t="inlineStr"/>
@@ -1373,511 +1373,501 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>eft:palgyi-lh-npo</t>
+          <t>eft:punyasambhava</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>1-1</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>Palgyi Lhünpo</t>
-        </is>
-      </c>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>eft:sarvanyadeva</t>
+          <t>eft:palgyi-lh-npo</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="D48" t="inlineStr"/>
-      <c r="E48" t="n">
-        <v>5</v>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>1-1</t>
+        </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>sarvanyadeva</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>kha che'i mkhan po sarba dz+nyA de ba, 'mkhan po sarba dz+nyA de ba/', 'sarvajñādeva'</t>
-        </is>
-      </c>
+          <t>Palgyi Lhünpo</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>eft:vidyakaraprabha</t>
+          <t>eft:sarvanyadeva</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>vidyakaraprabha</t>
+          <t>sarvanyadeva</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>'rgya gar gyi mkhan po bid+yA ka ra pra b+ha', 'slob dpon bid+yA ka ra pra b+hA/', 'vidyākaraprabha'</t>
+          <t>kha che'i mkhan po sarba dz+nyA de ba, 'mkhan po sarba dz+nyA de ba/', 'sarvajñādeva'</t>
         </is>
       </c>
       <c r="H49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>eft:jinamitra</t>
+          <t>eft:vidyakaraprabha</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Jinamitra</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr"/>
+          <t>vidyakaraprabha</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>'rgya gar gyi mkhan po bid+yA ka ra pra b+ha', 'slob dpon bid+yA ka ra pra b+hA/', 'vidyākaraprabha'</t>
+        </is>
+      </c>
       <c r="H50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>eft:sakyasena</t>
+          <t>eft:jinamitra</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>sakyasena</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>{'P8213': ['rgya gar gyi mkhan po bid+yA ka ra sing ha', 'slob dpon bIr+ya sing+ha pra b+ha/', 'vīryakarasiṁha,vīryasiṁha'], 'P8182': ['zhu chen gyi lots+tsha ba ban de dpal brtsegs', 'ska ba dpal brtsegs/']}</t>
-        </is>
-      </c>
+          <t>Jinamitra</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>eft:jnanasiddhi</t>
+          <t>eft:sakyasena</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>?</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>jnanasiddhi</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr"/>
+          <t>sakyasena</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>{'P8213': ['rgya gar gyi mkhan po bid+yA ka ra sing ha', 'slob dpon bIr+ya sing+ha pra b+ha/', 'vīryakarasiṁha,vīryasiṁha'], 'P8182': ['zhu chen gyi lots+tsha ba ban de dpal brtsegs', 'ska ba dpal brtsegs/']}</t>
+        </is>
+      </c>
       <c r="H52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>eft:anandasri-s-</t>
+          <t>eft:jnanasiddhi</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="n">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>anandasri (s)</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>paN+Di ta chen po A nan+da shrI', 'paN+Di ta A nan+da shrI', 'Ānandaśrī'</t>
-        </is>
-      </c>
+          <t>jnanasiddhi</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>eft:kawa-paltsek-under-the-name-paltsek-raksita-</t>
+          <t>eft:anandasri-s-</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="n">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Kawa Paltsek (under the name Paltsek Rakṣita)</t>
+          <t>anandasri (s)</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>'zhu chen gyi lo tsa ba ban de dpal brtsegs rak+Shi ta', 'ska ba dpal brtsegs/'</t>
+          <t>paN+Di ta chen po A nan+da shrI', 'paN+Di ta A nan+da shrI', 'Ānandaśrī'</t>
         </is>
       </c>
       <c r="H54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>eft:yesh-d-</t>
+          <t>eft:kawa-paltsek-under-the-name-paltsek-raksita-</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="n">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Yeshé Dé</t>
+          <t>Kawa Paltsek (under the name Paltsek Rakṣita)</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>'zhu chen gyi lo ts+tsha ba ban de ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
+          <t>'zhu chen gyi lo tsa ba ban de dpal brtsegs rak+Shi ta', 'ska ba dpal brtsegs/'</t>
         </is>
       </c>
       <c r="H55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>eft:danasila</t>
+          <t>eft:yesh-d-</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="n">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Danaśila</t>
+          <t>Yeshé Dé</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>'dA na shI la', 'paN chen dA na shI la/', 'dānaśīla'</t>
+          <t>'zhu chen gyi lo ts+tsha ba ban de ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
         </is>
       </c>
       <c r="H56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>eft:t-vidyakarasimha</t>
+          <t>eft:danasila</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="n">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>t. Vidyākarasiṃha</t>
+          <t>Danaśila</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>'rgya gar gyi mkhan po bid+yA ka ra sing ha', 'slob dpon bIr+ya sing+ha pra b+ha/', 'vīryakarasiṁha,vīryasiṁha'</t>
+          <t>'dA na shI la', 'paN chen dA na shI la/', 'dānaśīla'</t>
         </is>
       </c>
       <c r="H57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>eft:yesh-nyingpo</t>
+          <t>eft:t-vidyakarasimha</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="n">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Yeshé Nyingpo</t>
+          <t>t. Vidyākarasiṃha</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>'lots+tsha ba ban de ye shes snying po', 'lo tsA ba ye shes snying po/', 'Jñānagarbha'</t>
+          <t>'rgya gar gyi mkhan po bid+yA ka ra sing ha', 'slob dpon bIr+ya sing+ha pra b+ha/', 'vīryakarasiṁha,vīryasiṁha'</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>eft:band-yesh-d-</t>
+          <t>eft:yesh-nyingpo</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Bandé Yeshé Dé</t>
+          <t>Yeshé Nyingpo</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>'zhu chen gyi lots+tsha ba ban de ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
+          <t>'lots+tsha ba ban de ye shes snying po', 'lo tsA ba ye shes snying po/', 'Jñānagarbha'</t>
         </is>
       </c>
       <c r="H59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>eft:leki-d-</t>
+          <t>eft:band-yesh-d-</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="n">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Leki Dé</t>
+          <t>Bandé Yeshé Dé</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>'lo ts+tsha ba ban de legs kyi sde', 'legs kyi sde/'</t>
+          <t>'zhu chen gyi lots+tsha ba ban de ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
         </is>
       </c>
       <c r="H60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>eft:surendrabodhi</t>
+          <t>eft:leki-d-</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="n">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Surendrabodhi</t>
+          <t>Leki Dé</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>'shI len dra bo d+hi', 'shI len+dra bo d+hi/', 'śīlendrabodhi'</t>
+          <t>'lo ts+tsha ba ban de legs kyi sde', 'legs kyi sde/'</t>
         </is>
       </c>
       <c r="H61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>eft:yesh-d-ye-shes-sde-</t>
+          <t>eft:surendrabodhi</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="n">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Yeshé Dé (ye shes sde)</t>
+          <t>Surendrabodhi</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>'zhu chen gyi lo tsA ba _ban de ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
+          <t>'shI len dra bo d+hi', 'shI len+dra bo d+hi/', 'śīlendrabodhi'</t>
         </is>
       </c>
       <c r="H62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>eft:srilendrabodhi</t>
+          <t>eft:yesh-d-ye-shes-sde-</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="n">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Śrīlendrabodhi</t>
+          <t>Yeshé Dé (ye shes sde)</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>'rgya gar gyi mkhan po shI len dra bo d+hi', 'shI len+dra bo d+hi/', 'śīlendrabodhi'</t>
+          <t>'zhu chen gyi lo tsA ba _ban de ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
         </is>
       </c>
       <c r="H63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>eft:silendrabodhi</t>
+          <t>eft:srilendrabodhi</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1887,135 +1877,139 @@
       </c>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="n">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Śilendrabodhi</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr"/>
+          <t>Śrīlendrabodhi</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>'rgya gar gyi mkhan po shI len dra bo d+hi', 'shI len+dra bo d+hi/', 'śīlendrabodhi'</t>
+        </is>
+      </c>
       <c r="H64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>eft:dipamkarasrijnana</t>
+          <t>eft:silendrabodhi</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="n">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Dīpaṃkaraśrījñāna</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>'rgya gar gyi mkhan po dI paM ka ra shrI dz+nyA na', 'slob dpon mar med mdzad bzang po/', 'dīpaṁkaraśrijñāna,atīśa'</t>
-        </is>
-      </c>
+          <t>Śilendrabodhi</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>eft:prajnavarma</t>
+          <t>eft:dipamkarasrijnana</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="n">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>prajnavarma</t>
+          <t>Dīpaṃkaraśrījñāna</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>'pradz+nyA bad+ma', 'slob dpon shes rab go cha/', 'prajñāvarman'</t>
+          <t>'rgya gar gyi mkhan po dI paM ka ra shrI dz+nyA na', 'slob dpon mar med mdzad bzang po/', 'dīpaṁkaraśrijñāna,atīśa'</t>
         </is>
       </c>
       <c r="H66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>eft:dharmapala</t>
+          <t>eft:prajnavarma</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="n">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Dharmapāla</t>
+          <t>prajnavarma</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>'d+harma pA la', 'dpal ldan chos skyong /'</t>
+          <t>'pradz+nyA bad+ma', 'slob dpon shes rab go cha/', 'prajñāvarman'</t>
         </is>
       </c>
       <c r="H67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>eft:t-jnanagarbha</t>
+          <t>eft:dharmapala</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="n">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>t. Jñānagarbha</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr"/>
+          <t>Dharmapāla</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>'d+harma pA la', 'dpal ldan chos skyong /'</t>
+        </is>
+      </c>
       <c r="H68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -2024,7 +2018,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="D69" t="inlineStr"/>
@@ -2036,80 +2030,76 @@
           <t>t. Jñānagarbha</t>
         </is>
       </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>{'P8217': ['rgya gar gyi mkhan po dz+nyA na gar b+ha', 'dz+nyA na gar b+ha/', 'jñānagarbha ?'], 'P4255': ['lots+tsha ba ban+de ye shes snying po', 'lo tsA ba ye shes snying po/', 'Jñānagarbha']</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>Note: this is ambiguous. I wonder if the BDRC entries refer to different people (one is Sanskrit, the other is Tibetan, but they translate to each other)</t>
-        </is>
-      </c>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>eft:vidyakarasimha</t>
+          <t>eft:t-jnanagarbha</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="n">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Vidyākarasiṃha</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr"/>
-      <c r="H70" t="inlineStr"/>
+          <t>t. Jñānagarbha</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>{'P8217': ['rgya gar gyi mkhan po dz+nyA na gar b+ha', 'dz+nyA na gar b+ha/', 'jñānagarbha ?'], 'P4255': ['lots+tsha ba ban+de ye shes snying po', 'lo tsA ba ye shes snying po/', 'Jñānagarbha']</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Note: this is ambiguous. I wonder if the BDRC entries refer to different people (one is Sanskrit, the other is Tibetan, but they translate to each other)</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>eft:dharmatasila</t>
+          <t>eft:vidyakarasimha</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="n">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Dharmatāśila</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>'zhu chen gyi lots+tsha ba ban de d+harma tA shI la', 'zhu chen gyi lo tsA ba dharma tA shI la/', 'Dharmatāśīla'</t>
-        </is>
-      </c>
+          <t>Vidyākarasiṃha</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>eft:ch-nyi-tsultrim</t>
+          <t>eft:dharmatasila</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2119,499 +2109,529 @@
       </c>
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="n">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Chönyi Tsultrim</t>
+          <t>Dharmatāśila</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'lo ts+tsha ba ban de chos nyid tshul khrims', 'zhu chen gyi lo tsA ba dharma tA shI la/', 'Dharmatāśīla'</t>
+          <t>'zhu chen gyi lots+tsha ba ban de d+harma tA shI la', 'zhu chen gyi lo tsA ba dharma tA shI la/', 'Dharmatāśīla'</t>
         </is>
       </c>
       <c r="H72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>eft:jnanasidhi</t>
+          <t>eft:ch-nyi-tsultrim</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="n">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>jnanasidhi</t>
+          <t>Chönyi Tsultrim</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>'dz+nyA na sid+d+hi', 'dz+nyA na sid+dhi/', 'jñānasiddhi'</t>
+          <t xml:space="preserve"> 'lo ts+tsha ba ban de chos nyid tshul khrims', 'zhu chen gyi lo tsA ba dharma tA shI la/', 'Dharmatāśīla'</t>
         </is>
       </c>
       <c r="H73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>eft:paltsek</t>
+          <t>eft:jnanasidhi</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="n">
-        <v>225</v>
+        <v>178</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Paltsek</t>
+          <t>jnanasidhi</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>'zhu chen gyi lo ts+tsha ba ban de dpal brtsegs', 'ska ba dpal brtsegs/'</t>
+          <t>'dz+nyA na sid+d+hi', 'dz+nyA na sid+dhi/', 'jñānasiddhi'</t>
         </is>
       </c>
       <c r="H74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>eft:rinchen-tso</t>
+          <t>eft:paltsek</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="n">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Rinchen Tso</t>
+          <t>Paltsek</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>lo ts+tsha ba ban de rin chen 'tsho, "lo tsA ba rin chen 'tsho/"</t>
+          <t>'zhu chen gyi lo ts+tsha ba ban de dpal brtsegs', 'ska ba dpal brtsegs/'</t>
         </is>
       </c>
       <c r="H75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>eft:manjusrigarbha</t>
+          <t>eft:rinchen-tso</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="n">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Mañjuśrīgarbha</t>
+          <t>Rinchen Tso</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>'rgya gar gyi mkhan po many+dzu shrI gar+b+ha', 'mkhan po many+dzu shrI gar+b+ha/', 'majuśrīgarbha'</t>
+          <t>lo ts+tsha ba ban de rin chen 'tsho, "lo tsA ba rin chen 'tsho/"</t>
         </is>
       </c>
       <c r="H76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>eft:siladharma</t>
+          <t>eft:manjusrigarbha</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="n">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>siladharma</t>
+          <t>Mañjuśrīgarbha</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>{'P0TMPT007': ["rgya gar gyi d+harma rgya'i yi ge las ban de rnam par mi rtog", 'rnam par mi rtog pa']}</t>
+          <t>'rgya gar gyi mkhan po many+dzu shrI gar+b+ha', 'mkhan po many+dzu shrI gar+b+ha/', 'majuśrīgarbha'</t>
         </is>
       </c>
       <c r="H77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>eft:zhang-yesh-d-</t>
+          <t>eft:siladharma</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="n">
-        <v>309</v>
+        <v>242</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Zhang Yeshé Dé</t>
+          <t>siladharma</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>zhu chen gyi lo ts+tsha ba ban de zhang ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
+          <t>{'P0TMPT007': ["rgya gar gyi d+harma rgya'i yi ge las ban de rnam par mi rtog", 'rnam par mi rtog pa']}</t>
         </is>
       </c>
       <c r="H78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>eft:sherab-lekpa</t>
+          <t>eft:zhang-yesh-d-</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="n">
-        <v>349</v>
+        <v>309</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Sherab Lekpa</t>
+          <t>Zhang Yeshé Dé</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>'zhu chen gyi lots+tsha ba dge slong shes rab legs pa', 'shes rab legs pa/'</t>
+          <t>zhu chen gyi lo ts+tsha ba ban de zhang ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
         </is>
       </c>
       <c r="H79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>eft:sakya-yesh-</t>
+          <t>eft:sherab-lekpa</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="n">
-        <v>384</v>
+        <v>349</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Śākya Yeshé</t>
+          <t>Sherab Lekpa</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>'lots+tsha ba dge slong shAkya ye shes', 'brog mi lo tsA ba shAkya ye shes/'</t>
+          <t>'zhu chen gyi lots+tsha ba dge slong shes rab legs pa', 'shes rab legs pa/'</t>
         </is>
       </c>
       <c r="H80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>eft:jinavara</t>
+          <t>eft:sakya-yesh-</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="n">
-        <v>425</v>
+        <v>384</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Jinavara</t>
+          <t>Śākya Yeshé</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>'rgya gar gyi mkhan po dzi na bar', 'rgya gar gyi mkhan po dzi na bar', 'Jinapara'</t>
+          <t>'lots+tsha ba dge slong shAkya ye shes', 'brog mi lo tsA ba shAkya ye shes/'</t>
         </is>
       </c>
       <c r="H81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>eft:trakpa-gyaltsen</t>
+          <t>eft:jinavara</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="n">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Trakpa Gyaltsen</t>
+          <t>Jinavara</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>'lo ts+tsha ba grags pa rgyal mtshan', 'yar lung lo tsA ba grags pa rgyal mtshan/'</t>
+          <t>'rgya gar gyi mkhan po dzi na bar', 'rgya gar gyi mkhan po dzi na bar', 'Jinapara'</t>
         </is>
       </c>
       <c r="H82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>eft:phakpa-sherab</t>
+          <t>eft:trakpa-gyaltsen</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="n">
-        <v>498</v>
+        <v>431</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Phakpa Sherab</t>
+          <t>Trakpa Gyaltsen</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>bod kyi lo ts+tsha ba 'phags pa shes rab, "zangs dkar lo tsA ba 'phags pa shes rab/"</t>
+          <t>'lo ts+tsha ba grags pa rgyal mtshan', 'yar lung lo tsA ba grags pa rgyal mtshan/'</t>
         </is>
       </c>
       <c r="H83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>eft:kumarakalasa</t>
+          <t>eft:phakpa-sherab</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="n">
-        <v>543</v>
+        <v>498</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Kumārakalaśa</t>
+          <t>Phakpa Sherab</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>'rgya gar gyi mkhan po dge bsnyen chen po ku mA ra ka la sha', 'mkhan po gzhon nu bum pa/', 'kumārakalasa'</t>
+          <t>bod kyi lo ts+tsha ba 'phags pa shes rab, "zangs dkar lo tsA ba 'phags pa shes rab/"</t>
         </is>
       </c>
       <c r="H84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>eft:dipamkara-srijnana</t>
+          <t>eft:kumarakalasa</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="n">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Dīpaṃkara Śrījñāna</t>
+          <t>Kumārakalaśa</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>rgya gar gyi mkhan po chen po dI paM ka ra shrIdz+nyA na', 'slob dpon mar med mdzad bzang po/', 'dīpaṁkaraśrijñāna,atīśa'</t>
+          <t>'rgya gar gyi mkhan po dge bsnyen chen po ku mA ra ka la sha', 'mkhan po gzhon nu bum pa/', 'kumārakalasa'</t>
         </is>
       </c>
       <c r="H85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>eft:pa-tshab-nyi-ma-grags</t>
+          <t>eft:dipamkara-srijnana</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="n">
-        <v>850</v>
+        <v>544</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>pa tshab nyi ma grags</t>
+          <t>Dīpaṃkara Śrījñāna</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>'lo ts+tsha ba pa tsha ba nyi ma grags', 'pa tshab lo tsA ba nyi ma grags pa/'</t>
+          <t>rgya gar gyi mkhan po chen po dI paM ka ra shrIdz+nyA na', 'slob dpon mar med mdzad bzang po/', 'dīpaṁkaraśrijñāna,atīśa'</t>
         </is>
       </c>
       <c r="H86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>eft:band-yesh-de</t>
+          <t>eft:pa-tshab-nyi-ma-grags</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="D87" t="inlineStr"/>
       <c r="E87" t="n">
-        <v>725</v>
+        <v>850</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Bandé Yeshé De</t>
+          <t>pa tshab nyi ma grags</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>'zhu chen gyi lots+tsha ba ban+de ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
+          <t>'lo ts+tsha ba pa tsha ba nyi ma grags', 'pa tshab lo tsA ba nyi ma grags pa/'</t>
         </is>
       </c>
       <c r="H87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>eft:buddhakaravarma</t>
+          <t>eft:band-yesh-de</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="n">
+        <v>725</v>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Bandé Yeshé De</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>'zhu chen gyi lots+tsha ba ban+de ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>eft:buddhakaravarma</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>P8245</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr"/>
+      <c r="E89" t="n">
         <v>747</v>
       </c>
-      <c r="F88" t="inlineStr">
+      <c r="F89" t="inlineStr">
         <is>
           <t>Buddhākaravarma</t>
         </is>
       </c>
-      <c r="G88" t="inlineStr">
+      <c r="G89" t="inlineStr">
         <is>
           <t xml:space="preserve">'rgya gar gyi mkhan po bud+d+ha A ka ra ba rma', 'bud d+ha ka ra wa rman/', 'buddhakaravarman ?' </t>
         </is>
       </c>
-      <c r="H88" t="inlineStr"/>
+      <c r="H89" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2650,12 +2670,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -2665,12 +2685,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -2680,12 +2700,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -2695,12 +2715,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -2710,12 +2730,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -2725,12 +2745,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -2740,12 +2760,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
+          <t>{'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs'}</t>
         </is>
       </c>
     </row>
@@ -2755,12 +2775,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -2770,12 +2790,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -2785,12 +2805,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -2800,12 +2820,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2815,12 +2835,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
     </row>
@@ -2830,12 +2850,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
     </row>
@@ -2845,12 +2865,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -2860,12 +2880,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
     </row>
@@ -2875,12 +2895,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -2890,12 +2910,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -2905,12 +2925,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -2920,12 +2940,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -2935,12 +2955,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
     </row>
@@ -2965,12 +2985,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -2980,12 +3000,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -2995,12 +3015,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3010,12 +3030,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3025,12 +3045,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'eft:ye-shes-snying-po', 'eft:yesh-nyingpo', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3040,12 +3060,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3055,12 +3075,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -3070,12 +3090,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -3085,12 +3105,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3100,12 +3120,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -3115,12 +3135,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -3130,12 +3150,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -3145,12 +3165,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -3160,12 +3180,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P8210</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
         </is>
       </c>
     </row>
@@ -3175,12 +3195,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3190,12 +3210,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
     </row>
@@ -3205,12 +3225,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P8210</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3220,12 +3240,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -3235,12 +3255,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -3250,12 +3270,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
         </is>
       </c>
     </row>
@@ -3265,12 +3285,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -3280,12 +3300,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -3295,12 +3315,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -3310,12 +3330,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
     </row>
@@ -3325,12 +3345,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -3340,12 +3360,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -3355,12 +3375,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -3370,12 +3390,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3385,12 +3405,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po'}</t>
         </is>
       </c>
     </row>
@@ -3400,12 +3420,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -3415,12 +3435,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
         </is>
       </c>
     </row>
@@ -3430,12 +3450,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3445,12 +3465,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3460,12 +3480,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
incorporate new language attributions file
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -2670,12 +2670,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -2685,12 +2685,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -2700,12 +2700,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:ye-shes-snying-po', 'eft:yesh-nyingpo', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -2715,12 +2715,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -2730,12 +2730,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -2745,12 +2745,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
     </row>
@@ -2760,12 +2760,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -2775,12 +2775,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2790,12 +2790,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -2805,12 +2805,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -2820,12 +2820,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -2835,12 +2835,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2850,12 +2850,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -2865,12 +2865,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -2880,12 +2880,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -2895,12 +2895,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -2910,12 +2910,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -2925,12 +2925,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs'}</t>
         </is>
       </c>
     </row>
@@ -2940,12 +2940,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -2955,12 +2955,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -2970,12 +2970,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -2985,12 +2985,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -3000,12 +3000,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -3015,12 +3015,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
     </row>
@@ -3030,12 +3030,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -3045,12 +3045,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P8210</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:yesh-nyingpo', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3060,12 +3060,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -3075,12 +3075,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3090,12 +3090,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3105,12 +3105,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -3120,12 +3120,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3135,12 +3135,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
     </row>
@@ -3150,12 +3150,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -3165,12 +3165,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
     </row>
@@ -3180,12 +3180,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:band-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:zhang-yesh-d-'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -3195,12 +3195,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -3225,12 +3225,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P8210</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
         </is>
       </c>
     </row>
@@ -3255,12 +3255,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3270,12 +3270,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
+          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
     </row>
@@ -3285,12 +3285,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -3300,12 +3300,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -3315,12 +3315,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:silendrabodhi', 'eft:surendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3330,12 +3330,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -3345,12 +3345,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -3360,12 +3360,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:band-yesh-de', 'eft:ye-shes-sde', 'eft:band-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
         </is>
       </c>
     </row>
@@ -3375,12 +3375,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -3390,12 +3390,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
     </row>
@@ -3405,12 +3405,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -3420,12 +3420,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -3435,12 +3435,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
         </is>
       </c>
     </row>
@@ -3450,12 +3450,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -3465,12 +3465,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -3480,12 +3480,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add lang attribute when updating entries
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -2670,12 +2670,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
     </row>
@@ -2685,12 +2685,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -2700,12 +2700,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:yesh-nyingpo', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -2715,12 +2715,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
         </is>
       </c>
     </row>
@@ -2745,12 +2745,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -2760,12 +2760,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2775,12 +2775,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -2790,12 +2790,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -2805,12 +2805,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -2820,12 +2820,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -2835,12 +2835,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -2850,12 +2850,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -2865,12 +2865,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -2880,12 +2880,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
     </row>
@@ -2895,12 +2895,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -2910,12 +2910,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -2925,12 +2925,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs'}</t>
+          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -2940,12 +2940,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -2955,12 +2955,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -2970,12 +2970,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -2985,12 +2985,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -3000,12 +3000,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
         </is>
       </c>
     </row>
@@ -3015,12 +3015,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -3030,12 +3030,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -3045,12 +3045,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P8210</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -3060,12 +3060,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:zhang-yesh-d-', 'eft:band-yesh-d-', 'eft:band-yesh-de', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
         </is>
       </c>
     </row>
@@ -3075,12 +3075,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -3090,12 +3090,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3105,12 +3105,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
     </row>
@@ -3120,12 +3120,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:yesh-nyingpo', 'eft:t-jnanagarbha', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
     </row>
@@ -3135,12 +3135,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -3150,12 +3150,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3165,12 +3165,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -3180,12 +3180,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -3195,12 +3195,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -3210,12 +3210,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
+          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3225,12 +3225,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -3240,12 +3240,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -3255,12 +3255,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3270,12 +3270,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -3285,12 +3285,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3300,12 +3300,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3315,12 +3315,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi', 'eft:srilendrabodhi'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
     </row>
@@ -3330,12 +3330,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3345,12 +3345,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3360,12 +3360,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:band-yesh-de', 'eft:ye-shes-sde', 'eft:band-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs'}</t>
         </is>
       </c>
     </row>
@@ -3375,12 +3375,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P8210</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3390,12 +3390,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
         </is>
       </c>
     </row>
@@ -3405,12 +3405,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
     </row>
@@ -3420,12 +3420,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -3440,7 +3440,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
+          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
         </is>
       </c>
     </row>
@@ -3450,12 +3450,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -3465,12 +3465,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3480,12 +3480,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
find and add missing entries programatically
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -2670,12 +2670,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -2685,12 +2685,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs'}</t>
         </is>
       </c>
     </row>
@@ -2700,12 +2700,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
     </row>
@@ -2715,12 +2715,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2730,12 +2730,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
     </row>
@@ -2745,12 +2745,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -2760,12 +2760,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
     </row>
@@ -2775,12 +2775,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
         </is>
       </c>
     </row>
@@ -2790,12 +2790,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -2805,12 +2805,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -2820,12 +2820,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
     </row>
@@ -2835,12 +2835,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -2865,12 +2865,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
         </is>
       </c>
     </row>
@@ -2880,12 +2880,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -2895,12 +2895,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -2910,12 +2910,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
     </row>
@@ -2925,12 +2925,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2940,12 +2940,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -2955,12 +2955,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -2970,12 +2970,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -2985,12 +2985,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3000,12 +3000,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
     </row>
@@ -3015,12 +3015,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -3030,12 +3030,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -3045,12 +3045,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
         </is>
       </c>
     </row>
@@ -3060,12 +3060,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:zhang-yesh-d-', 'eft:band-yesh-d-', 'eft:band-yesh-de', 'eft:ye-shes-sde', 'eft:yesh-d-'}</t>
+          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -3075,12 +3075,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -3090,12 +3090,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -3105,12 +3105,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -3120,12 +3120,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:yesh-nyingpo', 'eft:t-jnanagarbha', 'eft:ye-shes-snying-po'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3135,12 +3135,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P8210</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3150,12 +3150,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3165,12 +3165,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -3180,12 +3180,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
     </row>
@@ -3195,12 +3195,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -3210,12 +3210,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -3225,12 +3225,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3240,12 +3240,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3255,12 +3255,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -3270,12 +3270,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3285,12 +3285,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:silendrabodhi', 'eft:surendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3300,12 +3300,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -3315,12 +3315,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -3330,12 +3330,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -3345,12 +3345,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -3360,12 +3360,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -3375,12 +3375,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P8210</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -3390,12 +3390,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -3405,12 +3405,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3420,12 +3420,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
         </is>
       </c>
     </row>
@@ -3435,12 +3435,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -3450,12 +3450,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -3465,12 +3465,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add langs from existing lang sheet
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -2690,12 +2690,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -2705,12 +2705,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
     </row>
@@ -2720,12 +2720,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -2735,12 +2735,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -2750,12 +2750,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
     </row>
@@ -2765,12 +2765,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -2780,12 +2780,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -2795,12 +2795,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
     </row>
@@ -2810,12 +2810,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -2825,12 +2825,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -2840,12 +2840,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -2855,12 +2855,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
         </is>
       </c>
     </row>
@@ -2870,12 +2870,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
         </is>
       </c>
     </row>
@@ -2885,12 +2885,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
         </is>
       </c>
     </row>
@@ -2900,12 +2900,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -2915,12 +2915,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -2930,12 +2930,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
     </row>
@@ -2945,12 +2945,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -2960,12 +2960,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
     </row>
@@ -2975,12 +2975,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -2990,12 +2990,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P8210</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3005,12 +3005,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -3020,12 +3020,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -3035,12 +3035,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3050,12 +3050,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -3065,12 +3065,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -3080,12 +3080,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3095,12 +3095,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:yesh-nyingpo', 'eft:ye-shes-snying-po', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3110,12 +3110,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -3125,12 +3125,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -3140,12 +3140,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3155,12 +3155,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -3170,12 +3170,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3185,12 +3185,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -3200,12 +3200,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -3215,12 +3215,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -3230,12 +3230,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:yesh-nyingpo', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3245,12 +3245,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -3260,12 +3260,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
     </row>
@@ -3275,12 +3275,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -3290,12 +3290,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -3305,12 +3305,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3320,12 +3320,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P8210</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:srilendrabodhi', 'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3335,12 +3335,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -3350,12 +3350,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -3365,12 +3365,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3380,12 +3380,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
     </row>
@@ -3395,12 +3395,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3410,12 +3410,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -3425,12 +3425,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3445,7 +3445,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
+          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
         </is>
       </c>
     </row>
@@ -3455,12 +3455,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -3470,12 +3470,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -3485,12 +3485,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -3500,12 +3500,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
revise attribution of languages
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -2690,12 +2690,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -2705,12 +2705,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -2720,12 +2720,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -2735,12 +2735,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
         </is>
       </c>
     </row>
@@ -2750,12 +2750,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:band-yesh-de', 'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -2765,12 +2765,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs'}</t>
         </is>
       </c>
     </row>
@@ -2780,7 +2780,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P8210</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -2795,12 +2795,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2810,12 +2810,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -2825,12 +2825,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -2840,12 +2840,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -2855,12 +2855,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -2870,12 +2870,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
     </row>
@@ -2885,12 +2885,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -2900,12 +2900,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -2915,12 +2915,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
         </is>
       </c>
     </row>
@@ -2930,12 +2930,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -2945,12 +2945,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -2960,12 +2960,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -2975,12 +2975,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -2990,12 +2990,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -3005,12 +3005,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
         </is>
       </c>
     </row>
@@ -3020,12 +3020,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -3035,12 +3035,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -3050,12 +3050,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3065,12 +3065,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
     </row>
@@ -3080,12 +3080,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
     </row>
@@ -3095,12 +3095,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:yesh-nyingpo', 'eft:ye-shes-snying-po', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
     </row>
@@ -3110,12 +3110,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -3125,12 +3125,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -3140,12 +3140,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -3155,12 +3155,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -3170,12 +3170,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -3185,12 +3185,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -3200,12 +3200,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -3215,12 +3215,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -3230,12 +3230,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -3245,12 +3245,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
     </row>
@@ -3260,12 +3260,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra'}</t>
+          <t>{'eft:silendrabodhi', 'eft:srilendrabodhi', 'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3275,12 +3275,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -3290,12 +3290,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -3305,12 +3305,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -3320,12 +3320,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P8210</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
     </row>
@@ -3335,12 +3335,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -3350,12 +3350,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3365,12 +3365,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -3380,12 +3380,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3395,12 +3395,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3410,12 +3410,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
     </row>
@@ -3425,12 +3425,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -3440,12 +3440,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -3455,12 +3455,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -3470,12 +3470,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
         </is>
       </c>
     </row>
@@ -3485,12 +3485,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3500,12 +3500,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
alter script to account for missing attributes, add more language attributes
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -722,7 +722,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>P8210</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -737,12 +737,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>eft:prajnavarman</t>
+          <t>eft:munivarman</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -757,12 +757,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>eft:dpal-dbyangs</t>
+          <t>eft:prajnavarman</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -777,12 +777,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>eft:ska-ba-dpal-brtsegs</t>
+          <t>eft:dpal-dbyangs</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
@@ -797,12 +797,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>eft:munivarman</t>
+          <t>eft:ska-ba-dpal-brtsegs</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
@@ -2664,7 +2664,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2690,12 +2690,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -2705,12 +2705,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -2735,12 +2735,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2750,12 +2750,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:zhang-yesh-d-', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de'}</t>
         </is>
       </c>
     </row>
@@ -2765,12 +2765,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2780,12 +2780,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P8210</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -2795,12 +2795,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -2810,12 +2810,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -2825,12 +2825,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -2840,12 +2840,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -2855,12 +2855,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -2870,12 +2870,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:band-yesh-de', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -2885,12 +2885,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -2900,12 +2900,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -2915,12 +2915,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
     </row>
@@ -2930,12 +2930,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
         </is>
       </c>
     </row>
@@ -2945,12 +2945,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -2960,12 +2960,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -2975,12 +2975,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -2990,12 +2990,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
     </row>
@@ -3005,12 +3005,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -3020,12 +3020,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3035,12 +3035,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3050,12 +3050,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -3065,12 +3065,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -3080,12 +3080,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3095,12 +3095,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -3110,12 +3110,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -3125,12 +3125,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3140,12 +3140,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:paltsek', 'eft:ban-de-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
         </is>
       </c>
     </row>
@@ -3155,12 +3155,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
     </row>
@@ -3170,12 +3170,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:srilendrabodhi', 'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3185,12 +3185,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3215,12 +3215,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -3230,12 +3230,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
     </row>
@@ -3245,12 +3245,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
     </row>
@@ -3260,12 +3260,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:srilendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
         </is>
       </c>
     </row>
@@ -3275,12 +3275,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -3290,12 +3290,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -3305,12 +3305,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -3320,12 +3320,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -3335,12 +3335,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -3350,12 +3350,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -3365,12 +3365,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
         </is>
       </c>
     </row>
@@ -3380,12 +3380,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -3395,12 +3395,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3410,12 +3410,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
     </row>
@@ -3425,12 +3425,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3440,12 +3440,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -3455,12 +3455,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -3470,12 +3470,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -3485,27 +3485,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>P8219</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix code to note existing attributions
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -2690,12 +2690,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -2705,12 +2705,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -2720,12 +2720,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -2735,12 +2735,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
     </row>
@@ -2750,12 +2750,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:band-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:zhang-yesh-d-', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2765,12 +2765,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -2780,12 +2780,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
     </row>
@@ -2795,12 +2795,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
     </row>
@@ -2810,12 +2810,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -2825,12 +2825,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
     </row>
@@ -2840,12 +2840,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:ye-shes-snying-po', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
     </row>
@@ -2855,12 +2855,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
         </is>
       </c>
     </row>
@@ -2870,12 +2870,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2900,12 +2900,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -2915,12 +2915,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -2930,12 +2930,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -2945,12 +2945,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -2960,12 +2960,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -2975,12 +2975,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -2990,12 +2990,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3005,12 +3005,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
         </is>
       </c>
     </row>
@@ -3035,12 +3035,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -3050,12 +3050,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -3065,12 +3065,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po'}</t>
         </is>
       </c>
     </row>
@@ -3080,12 +3080,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
     </row>
@@ -3095,12 +3095,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -3125,12 +3125,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
         </is>
       </c>
     </row>
@@ -3140,12 +3140,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:paltsek', 'eft:ban-de-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -3155,12 +3155,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -3170,12 +3170,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:srilendrabodhi', 'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -3185,12 +3185,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -3200,12 +3200,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -3215,12 +3215,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -3230,12 +3230,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -3245,12 +3245,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
     </row>
@@ -3260,12 +3260,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3275,12 +3275,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -3290,12 +3290,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3305,12 +3305,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -3320,12 +3320,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -3335,12 +3335,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
     </row>
@@ -3350,12 +3350,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3365,12 +3365,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3380,12 +3380,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -3395,12 +3395,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3410,12 +3410,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -3425,12 +3425,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -3440,12 +3440,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -3455,12 +3455,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3470,12 +3470,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3485,12 +3485,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
collect attributions to add and add them to spreadsheet
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -2690,12 +2690,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
     </row>
@@ -2705,12 +2705,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -2720,12 +2720,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -2735,12 +2735,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -2750,12 +2750,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
         </is>
       </c>
     </row>
@@ -2765,12 +2765,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -2780,12 +2780,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -2795,12 +2795,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -2810,12 +2810,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -2825,12 +2825,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
         </is>
       </c>
     </row>
@@ -2840,12 +2840,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:ye-shes-snying-po', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -2855,12 +2855,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -2870,12 +2870,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -2885,12 +2885,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:band-yesh-de', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
     </row>
@@ -2900,12 +2900,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -2915,12 +2915,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -2930,12 +2930,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -2945,12 +2945,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -2960,12 +2960,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -2975,12 +2975,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -2990,12 +2990,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -3005,12 +3005,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3020,12 +3020,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -3035,12 +3035,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -3050,12 +3050,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
+          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
     </row>
@@ -3065,12 +3065,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3080,12 +3080,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -3095,12 +3095,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -3110,12 +3110,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -3125,12 +3125,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
         </is>
       </c>
     </row>
@@ -3140,12 +3140,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3155,12 +3155,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3170,12 +3170,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -3185,12 +3185,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -3200,12 +3200,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -3215,12 +3215,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3230,12 +3230,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3245,12 +3245,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -3260,12 +3260,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -3275,12 +3275,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
         </is>
       </c>
     </row>
@@ -3290,12 +3290,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -3305,12 +3305,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -3320,12 +3320,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:silendrabodhi', 'eft:srilendrabodhi', 'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3335,12 +3335,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -3350,12 +3350,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
         </is>
       </c>
     </row>
@@ -3365,12 +3365,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3380,12 +3380,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -3395,12 +3395,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
         </is>
       </c>
     </row>
@@ -3410,12 +3410,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -3425,12 +3425,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -3440,12 +3440,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -3455,12 +3455,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
         </is>
       </c>
     </row>
@@ -3470,12 +3470,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
     </row>
@@ -3485,12 +3485,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
try to find bdrc match for existing attributions
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -2690,12 +2690,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -2705,12 +2705,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -2720,12 +2720,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
         </is>
       </c>
     </row>
@@ -2735,12 +2735,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2750,12 +2750,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -2765,12 +2765,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -2780,12 +2780,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -2795,12 +2795,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -2810,12 +2810,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -2825,12 +2825,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -2840,12 +2840,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
     </row>
@@ -2855,12 +2855,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
     </row>
@@ -2870,12 +2870,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-'}</t>
         </is>
       </c>
     </row>
@@ -2885,12 +2885,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:band-yesh-de', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -2900,12 +2900,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -2915,12 +2915,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -2930,12 +2930,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -2945,12 +2945,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -2960,12 +2960,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -2975,12 +2975,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -2990,12 +2990,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
     </row>
@@ -3005,12 +3005,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3020,12 +3020,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3035,12 +3035,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3050,12 +3050,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -3065,12 +3065,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3080,12 +3080,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -3095,12 +3095,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -3110,12 +3110,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3125,12 +3125,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -3140,12 +3140,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
     </row>
@@ -3155,12 +3155,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
+          <t>{'eft:yesh-nyingpo', 'eft:ye-shes-snying-po', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3170,12 +3170,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3185,12 +3185,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -3200,12 +3200,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -3215,12 +3215,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -3230,12 +3230,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3245,12 +3245,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -3260,12 +3260,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -3275,12 +3275,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -3290,12 +3290,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
     </row>
@@ -3305,12 +3305,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -3320,12 +3320,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:srilendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
     </row>
@@ -3335,12 +3335,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -3350,12 +3350,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -3365,12 +3365,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
     </row>
@@ -3380,12 +3380,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
     </row>
@@ -3395,12 +3395,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -3410,12 +3410,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -3425,12 +3425,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -3440,12 +3440,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -3455,12 +3455,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -3470,12 +3470,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
         </is>
       </c>
     </row>
@@ -3485,12 +3485,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix matching of hyphenated attributions
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -2690,12 +2690,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -2705,12 +2705,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -2720,12 +2720,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
     </row>
@@ -2735,12 +2735,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -2750,12 +2750,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -2765,12 +2765,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -2780,12 +2780,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -2795,12 +2795,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -2810,12 +2810,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -2825,12 +2825,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -2840,12 +2840,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -2855,12 +2855,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -2870,12 +2870,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -2885,12 +2885,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -2900,12 +2900,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2930,12 +2930,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -2945,12 +2945,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -2960,12 +2960,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -2975,12 +2975,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -2990,12 +2990,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -3005,12 +3005,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -3020,12 +3020,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:ye-shes-snying-po', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
     </row>
@@ -3035,12 +3035,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -3065,12 +3065,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
     </row>
@@ -3080,12 +3080,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -3095,12 +3095,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -3110,12 +3110,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
     </row>
@@ -3125,12 +3125,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
     </row>
@@ -3140,12 +3140,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3155,12 +3155,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:yesh-nyingpo', 'eft:ye-shes-snying-po', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -3170,12 +3170,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3185,12 +3185,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -3200,12 +3200,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
         </is>
       </c>
     </row>
@@ -3215,12 +3215,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -3230,12 +3230,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
         </is>
       </c>
     </row>
@@ -3260,12 +3260,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3275,12 +3275,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3290,12 +3290,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -3305,12 +3305,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -3320,12 +3320,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -3335,12 +3335,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3350,12 +3350,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
     </row>
@@ -3365,12 +3365,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3380,12 +3380,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -3395,12 +3395,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po'}</t>
         </is>
       </c>
     </row>
@@ -3410,12 +3410,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -3425,12 +3425,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-'}</t>
         </is>
       </c>
     </row>
@@ -3440,12 +3440,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
         </is>
       </c>
     </row>
@@ -3455,12 +3455,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
     </row>
@@ -3470,12 +3470,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -3485,12 +3485,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
remove unknown from uris
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -2690,12 +2690,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -2705,12 +2705,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -2720,12 +2720,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
         </is>
       </c>
     </row>
@@ -2735,12 +2735,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de'}</t>
         </is>
       </c>
     </row>
@@ -2750,12 +2750,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -2765,12 +2765,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -2780,12 +2780,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -2795,12 +2795,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -2810,12 +2810,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -2825,12 +2825,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
         </is>
       </c>
     </row>
@@ -2840,12 +2840,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -2855,12 +2855,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -2870,12 +2870,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -2885,12 +2885,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -2900,12 +2900,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -2915,12 +2915,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -2930,12 +2930,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -2945,12 +2945,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
     </row>
@@ -2960,12 +2960,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
         </is>
       </c>
     </row>
@@ -2975,12 +2975,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -2990,12 +2990,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3005,12 +3005,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
         </is>
       </c>
     </row>
@@ -3020,12 +3020,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:ye-shes-snying-po', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -3050,12 +3050,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:srilendrabodhi', 'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3065,12 +3065,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -3080,12 +3080,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -3095,12 +3095,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -3110,12 +3110,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
     </row>
@@ -3125,12 +3125,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3140,12 +3140,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3155,12 +3155,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -3170,12 +3170,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:srilendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3185,12 +3185,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -3200,12 +3200,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -3215,12 +3215,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -3230,12 +3230,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -3245,12 +3245,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -3260,12 +3260,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
     </row>
@@ -3275,12 +3275,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -3290,12 +3290,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3305,12 +3305,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
     </row>
@@ -3320,12 +3320,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -3335,12 +3335,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -3350,12 +3350,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3365,12 +3365,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3380,12 +3380,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -3395,12 +3395,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -3410,12 +3410,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
         </is>
       </c>
     </row>
@@ -3425,12 +3425,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -3440,12 +3440,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -3455,12 +3455,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
     </row>
@@ -3470,12 +3470,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
     </row>
@@ -3485,12 +3485,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
strip out question mark
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -2690,12 +2690,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -2705,12 +2705,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -2720,12 +2720,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
     </row>
@@ -2735,12 +2735,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2750,12 +2750,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:srilendrabodhi', 'eft:silendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -2765,12 +2765,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:srilendrabodhi', 'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -2785,7 +2785,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
+          <t>{'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
     </row>
@@ -2795,12 +2795,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -2810,12 +2810,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -2825,12 +2825,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
         </is>
       </c>
     </row>
@@ -2840,12 +2840,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -2855,12 +2855,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -2870,12 +2870,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -2885,12 +2885,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -2900,12 +2900,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -2915,12 +2915,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -2930,12 +2930,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
     </row>
@@ -2945,12 +2945,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
         </is>
       </c>
     </row>
@@ -2960,12 +2960,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
         </is>
       </c>
     </row>
@@ -2975,12 +2975,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -2990,12 +2990,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3005,12 +3005,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -3020,12 +3020,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3035,12 +3035,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -3050,12 +3050,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -3065,12 +3065,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -3080,12 +3080,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3095,12 +3095,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -3110,12 +3110,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -3140,12 +3140,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -3155,12 +3155,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
         </is>
       </c>
     </row>
@@ -3170,12 +3170,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:yesh-nyingpo', 'eft:ye-shes-snying-po', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3185,12 +3185,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -3200,12 +3200,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -3215,12 +3215,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:yesh-d-', 'eft:ye-shes-sde'}</t>
         </is>
       </c>
     </row>
@@ -3230,12 +3230,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -3245,12 +3245,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -3260,12 +3260,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3275,12 +3275,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -3290,12 +3290,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -3310,7 +3310,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
     </row>
@@ -3320,12 +3320,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -3335,12 +3335,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3350,12 +3350,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -3365,12 +3365,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
+          <t>{'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra'}</t>
         </is>
       </c>
     </row>
@@ -3380,12 +3380,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -3395,12 +3395,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
     </row>
@@ -3410,12 +3410,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -3425,12 +3425,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -3440,12 +3440,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-', 'eft:jinamitra'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -3455,12 +3455,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -3470,12 +3470,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -3485,12 +3485,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add lang attribute to label element
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -2690,12 +2690,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
     </row>
@@ -2705,12 +2705,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -2720,12 +2720,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po'}</t>
         </is>
       </c>
     </row>
@@ -2735,12 +2735,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -2750,12 +2750,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -2770,7 +2770,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:srilendrabodhi', 'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:silendrabodhi', 'eft:srilendrabodhi', 'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -2780,12 +2780,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -2795,12 +2795,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -2810,12 +2810,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -2825,12 +2825,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -2840,12 +2840,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
         </is>
       </c>
     </row>
@@ -2870,12 +2870,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2885,12 +2885,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -2900,12 +2900,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -2915,12 +2915,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -2930,12 +2930,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -2945,12 +2945,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -2960,12 +2960,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:paltsek', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
     </row>
@@ -2975,12 +2975,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
     </row>
@@ -2990,12 +2990,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -3005,12 +3005,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -3020,12 +3020,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -3035,12 +3035,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -3050,12 +3050,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -3065,12 +3065,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -3080,12 +3080,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -3095,12 +3095,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3110,12 +3110,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -3125,12 +3125,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -3140,12 +3140,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3155,12 +3155,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -3170,12 +3170,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:yesh-nyingpo', 'eft:ye-shes-snying-po', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
     </row>
@@ -3185,12 +3185,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3200,12 +3200,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -3215,12 +3215,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:band-yesh-de', 'eft:band-yesh-d-', 'eft:zhang-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:yesh-d-', 'eft:ye-shes-sde'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -3230,12 +3230,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3245,12 +3245,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -3260,12 +3260,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -3275,12 +3275,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3290,12 +3290,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3305,12 +3305,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -3320,12 +3320,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
         </is>
       </c>
     </row>
@@ -3335,12 +3335,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3350,12 +3350,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3365,12 +3365,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra'}</t>
+          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:band-yesh-d-'}</t>
         </is>
       </c>
     </row>
@@ -3380,12 +3380,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
     </row>
@@ -3400,7 +3400,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
     </row>
@@ -3410,12 +3410,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -3425,12 +3425,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -3440,12 +3440,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
     </row>
@@ -3455,12 +3455,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
         </is>
       </c>
     </row>
@@ -3470,12 +3470,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
strip out extraneous marks from BDRC ID's
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -2690,12 +2690,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -2705,12 +2705,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -2720,12 +2720,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -2735,12 +2735,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -2750,12 +2750,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -2765,12 +2765,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:srilendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -2780,12 +2780,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -2795,12 +2795,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
         </is>
       </c>
     </row>
@@ -2810,12 +2810,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -2825,12 +2825,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -2840,12 +2840,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
     </row>
@@ -2855,12 +2855,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -2870,12 +2870,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -2885,12 +2885,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
     </row>
@@ -2900,12 +2900,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
     </row>
@@ -2915,12 +2915,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2930,12 +2930,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -2945,12 +2945,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -2960,12 +2960,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:paltsek', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -2975,12 +2975,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -2990,12 +2990,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3005,12 +3005,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3020,12 +3020,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -3035,12 +3035,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -3050,12 +3050,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -3065,12 +3065,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
     </row>
@@ -3080,12 +3080,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-de', 'eft:band-yesh-d-'}</t>
         </is>
       </c>
     </row>
@@ -3095,12 +3095,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek'}</t>
         </is>
       </c>
     </row>
@@ -3110,12 +3110,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -3125,12 +3125,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -3140,12 +3140,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -3155,12 +3155,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
         </is>
       </c>
     </row>
@@ -3170,12 +3170,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3185,12 +3185,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -3200,12 +3200,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3215,12 +3215,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3230,12 +3230,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -3245,12 +3245,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -3260,12 +3260,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3275,12 +3275,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -3290,12 +3290,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -3305,12 +3305,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3320,12 +3320,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3335,12 +3335,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -3350,12 +3350,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
         </is>
       </c>
     </row>
@@ -3365,12 +3365,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:band-yesh-d-'}</t>
+          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
     </row>
@@ -3380,12 +3380,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
         </is>
       </c>
     </row>
@@ -3395,12 +3395,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -3410,12 +3410,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -3425,12 +3425,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -3440,12 +3440,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3455,12 +3455,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
         </is>
       </c>
     </row>
@@ -3470,12 +3470,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -3485,12 +3485,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add more attributions from 84000 XML, for texts with some  existing BDRC data
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2652,6 +2652,318 @@
         </is>
       </c>
       <c r="H90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Gö Chödrup</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr"/>
+      <c r="E91" t="inlineStr"/>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>eft:g-ch-drup</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr"/>
+      <c r="H91" t="inlineStr"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>wang phab zhwun (wang phan zhun)</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr"/>
+      <c r="E92" t="inlineStr"/>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>eft:wang-phab-zhwun-wang-phan-zhun-</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr"/>
+      <c r="H92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>dge ba'i blo gros</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr"/>
+      <c r="E93" t="inlineStr"/>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>eft:dge-ba-i-blo-gros</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr"/>
+      <c r="H93" t="inlineStr"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>rgya mtsho'i sde</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr"/>
+      <c r="E94" t="inlineStr"/>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>eft:rgya-mtsho-i-sde</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr"/>
+      <c r="H94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Thönmi Sambhoṭa</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr"/>
+      <c r="E95" t="inlineStr"/>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>eft:th-nmi-sambhota</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr"/>
+      <c r="H95" t="inlineStr"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Tsultrim Gyaltsen</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr"/>
+      <c r="E96" t="inlineStr"/>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>eft:tsultrim-gyaltsen</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr"/>
+      <c r="H96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Shang Buchikpa</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr"/>
+      <c r="E97" t="inlineStr"/>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>eft:shang-buchikpa</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr"/>
+      <c r="H97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Sherap Ö</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr"/>
+      <c r="E98" t="inlineStr"/>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>eft:sherap-</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr"/>
+      <c r="H98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Paṇḍita Dharmākara</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr"/>
+      <c r="E99" t="inlineStr"/>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>eft:pandita-dharmakara</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr"/>
+      <c r="H99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Lotsāwa Zangkyong (bzang skyong)</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr"/>
+      <c r="E100" t="inlineStr"/>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>eft:lotsawa-zangkyong-bzang-skyong-</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr"/>
+      <c r="H100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Nyen Lotsawa Darma Drak</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr"/>
+      <c r="E101" t="inlineStr"/>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>eft:nyen-lotsawa-darma-drak</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr"/>
+      <c r="H101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Patsap Nyima Drak [?]</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr"/>
+      <c r="E102" t="inlineStr"/>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>eft:patsap-nyima-drak-</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr"/>
+      <c r="H102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>vajrvisramitra</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr"/>
+      <c r="E103" t="inlineStr"/>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>eft:vajrvisramitra</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr"/>
+      <c r="H103" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2690,12 +3002,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -2705,12 +3017,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -2720,12 +3032,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -2735,12 +3047,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -2750,12 +3062,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
         </is>
       </c>
     </row>
@@ -2765,12 +3077,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -2780,12 +3092,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -2795,12 +3107,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -2810,12 +3122,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
     </row>
@@ -2825,12 +3137,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -2840,12 +3152,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -2855,12 +3167,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -2870,12 +3182,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -2885,12 +3197,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'Shang Buchikpa', 'Patsap Nyima Drak [?]', 'vajrvisramitra', 'Thönmi Sambhoṭa', 'Sherap Ö', 'wang phab zhwun (wang phan zhun)', 'Gö Chödrup', "dge ba'i blo gros", 'Lotsāwa Zangkyong (bzang skyong)', 'Tsultrim Gyaltsen', 'Paṇḍita Dharmākara', 'Nyen Lotsawa Darma Drak', 'eft:sakyasena', "rgya mtsho'i sde"}</t>
         </is>
       </c>
     </row>
@@ -2900,12 +3212,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -2915,12 +3227,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -2930,12 +3242,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -2945,12 +3257,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -2960,12 +3272,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -2975,12 +3287,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
     </row>
@@ -2990,12 +3302,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -3005,12 +3317,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -3020,12 +3332,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3035,12 +3347,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
+          <t>{'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -3065,12 +3377,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -3080,12 +3392,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-ye-shes-sde-', 'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-de', 'eft:band-yesh-d-'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
     </row>
@@ -3095,12 +3407,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3110,12 +3422,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -3125,12 +3437,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3140,12 +3452,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -3155,12 +3467,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
+          <t>{'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
         </is>
       </c>
     </row>
@@ -3170,12 +3482,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3185,12 +3497,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -3200,12 +3512,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
         </is>
       </c>
     </row>
@@ -3215,12 +3527,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -3230,12 +3542,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -3245,12 +3557,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
     </row>
@@ -3260,12 +3572,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
+          <t>{'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -3275,12 +3587,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -3290,12 +3602,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -3305,12 +3617,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3320,12 +3632,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
     </row>
@@ -3335,12 +3647,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
         </is>
       </c>
     </row>
@@ -3350,12 +3662,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
     </row>
@@ -3365,12 +3677,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
+          <t>{'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -3380,12 +3692,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -3395,12 +3707,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -3410,12 +3722,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -3425,12 +3737,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3440,12 +3752,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
     </row>
@@ -3455,12 +3767,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -3470,12 +3782,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
     </row>
@@ -3485,12 +3797,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add new data on person identifications
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H103"/>
+  <dimension ref="A1:H124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2664,7 +2664,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8221</t>
         </is>
       </c>
       <c r="D91" t="inlineStr"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8276</t>
         </is>
       </c>
       <c r="D92" t="inlineStr"/>
@@ -2712,7 +2712,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8278</t>
         </is>
       </c>
       <c r="D93" t="inlineStr"/>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8277</t>
         </is>
       </c>
       <c r="D94" t="inlineStr"/>
@@ -2760,7 +2760,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P5788</t>
         </is>
       </c>
       <c r="D95" t="inlineStr"/>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P6453</t>
         </is>
       </c>
       <c r="D96" t="inlineStr"/>
@@ -2808,7 +2808,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P1321</t>
         </is>
       </c>
       <c r="D97" t="inlineStr"/>
@@ -2856,7 +2856,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="D99" t="inlineStr"/>
@@ -2880,7 +2880,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P4256</t>
         </is>
       </c>
       <c r="D100" t="inlineStr"/>
@@ -2904,7 +2904,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P2614</t>
         </is>
       </c>
       <c r="D101" t="inlineStr"/>
@@ -2928,7 +2928,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="D102" t="inlineStr"/>
@@ -2964,6 +2964,514 @@
       </c>
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>bidyakaraprabha</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>P8211</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr"/>
+      <c r="E104" t="inlineStr"/>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>eft:bidyakaraprabha</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr"/>
+      <c r="H104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>subhasita</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>P8280</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr"/>
+      <c r="E105" t="inlineStr"/>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>eft:subhasita</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr"/>
+      <c r="H105" t="inlineStr"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>rin chen bzag po</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>P753</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr"/>
+      <c r="E106" t="inlineStr"/>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>eft:rin-chen-bzag-po</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>this is a typo, not a different person</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>'brom rgyal ba'i 'byung gnas</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>P2557</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr"/>
+      <c r="E107" t="inlineStr"/>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>eft:-brom-rgyal-ba-i-byung-gnas</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr"/>
+      <c r="H107" t="inlineStr"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>'brom</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>P2557</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr"/>
+      <c r="E108" t="inlineStr"/>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>eft:-brom</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr"/>
+      <c r="H108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>blo ldan shes rab</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>P2551</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr"/>
+      <c r="E109" t="inlineStr"/>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>eft:blo-ldan-shes-rab</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr"/>
+      <c r="H109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Yeshé De</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>P8205</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr"/>
+      <c r="E110" t="inlineStr"/>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>eft:yesh-de</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr"/>
+      <c r="H110" t="inlineStr"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Lotsawa Bandé Dharmatāśīla</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>P8266</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr"/>
+      <c r="E111" t="inlineStr"/>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>eft:lotsawa-band-dharmatasila</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr"/>
+      <c r="H111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Gewai Lodrö</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>P8278</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr"/>
+      <c r="E112" t="inlineStr"/>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>eft:gewai-lodr-</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr"/>
+      <c r="H112" t="inlineStr"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Devendrarakṣita</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>P8212</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr"/>
+      <c r="E113" t="inlineStr"/>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>eft:devendraraksita</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr"/>
+      <c r="H113" t="inlineStr"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Kumārarakṣita</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>P8271</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr"/>
+      <c r="E114" t="inlineStr"/>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>eft:kumararaksita</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr"/>
+      <c r="H114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Gewé Pal</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>P4263</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr"/>
+      <c r="E115" t="inlineStr"/>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>eft:gew-pal</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr"/>
+      <c r="H115" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Bandé Paltsek</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>P8182</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr"/>
+      <c r="E116" t="inlineStr"/>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>eft:band-paltsek</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr"/>
+      <c r="H116" t="inlineStr"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Rinchen Zangpo</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>P753</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr"/>
+      <c r="E117" t="inlineStr"/>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>eft:rinchen-zangpo</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr"/>
+      <c r="H117" t="inlineStr"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Gö Lhetsé</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>P3458</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr"/>
+      <c r="E118" t="inlineStr"/>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>eft:g-lhets-</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr"/>
+      <c r="H118" t="inlineStr"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Śākya Lodrö</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>P8216</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr"/>
+      <c r="E119" t="inlineStr"/>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>eft:sakya-lodr-</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr"/>
+      <c r="H119" t="inlineStr"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Géwai Lodrö</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>P1242</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr"/>
+      <c r="E120" t="inlineStr"/>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>eft:g-wai-lodr-</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr"/>
+      <c r="H120" t="inlineStr"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Tsultrim Gyalwa</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>P3456</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr"/>
+      <c r="E121" t="inlineStr"/>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>eft:tsultrim-gyalwa</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr"/>
+      <c r="H121" t="inlineStr"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Patsap Nyima Drak [?]</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>P5651</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr"/>
+      <c r="E122" t="inlineStr"/>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>eft:patsap-nyima-drak-</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr"/>
+      <c r="H122" t="inlineStr"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Chökyi Sherab</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>P3890</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr"/>
+      <c r="E123" t="inlineStr"/>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>eft:ch-kyi-sherab</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr"/>
+      <c r="H123" t="inlineStr"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>vairocanaraksita</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>P4CZ15308</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr"/>
+      <c r="E124" t="inlineStr"/>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>eft:vairocanaraksita</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr"/>
+      <c r="H124" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2976,7 +3484,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3002,12 +3510,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
+          <t>{'Gewé Pal', 'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -3017,12 +3525,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P8278</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'Gewai Lodrö', "dge ba'i blo gros"}</t>
         </is>
       </c>
     </row>
@@ -3032,12 +3540,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:dpal-brtsegs', 'Bandé Paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
         </is>
       </c>
     </row>
@@ -3047,12 +3555,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:dharmatasila', 'Lotsawa Bandé Dharmatāśīla', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
     </row>
@@ -3062,12 +3570,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P8221</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
+          <t>{'Gö Chödrup'}</t>
         </is>
       </c>
     </row>
@@ -3077,12 +3585,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-', 'eft:zhang-yesh-d-', 'eft:yesh-d-', 'eft:band-yesh-d-', 'Yeshé De', 'eft:band-yesh-de'}</t>
         </is>
       </c>
     </row>
@@ -3092,12 +3600,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'Patsap Nyima Drak [?]', 'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -3107,12 +3615,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P4CZ15308</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'vairocanaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3122,12 +3630,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -3137,12 +3645,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -3152,12 +3660,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
         </is>
       </c>
     </row>
@@ -3167,12 +3675,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3182,12 +3690,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P5788</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'Thönmi Sambhoṭa'}</t>
         </is>
       </c>
     </row>
@@ -3197,12 +3705,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'Shang Buchikpa', 'Patsap Nyima Drak [?]', 'vajrvisramitra', 'Thönmi Sambhoṭa', 'Sherap Ö', 'wang phab zhwun (wang phan zhun)', 'Gö Chödrup', "dge ba'i blo gros", 'Lotsāwa Zangkyong (bzang skyong)', 'Tsultrim Gyaltsen', 'Paṇḍita Dharmākara', 'Nyen Lotsawa Darma Drak', 'eft:sakyasena', "rgya mtsho'i sde"}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -3212,12 +3720,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
     </row>
@@ -3227,12 +3735,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -3242,12 +3750,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -3257,12 +3765,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -3272,12 +3780,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P3890</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'Chökyi Sherab'}</t>
         </is>
       </c>
     </row>
@@ -3287,12 +3795,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3302,12 +3810,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P8276</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha'}</t>
+          <t>{'wang phab zhwun (wang phan zhun)'}</t>
         </is>
       </c>
     </row>
@@ -3317,12 +3825,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
         </is>
       </c>
     </row>
@@ -3332,12 +3840,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -3347,12 +3855,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -3362,12 +3870,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P8277</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{"rgya mtsho'i sde"}</t>
         </is>
       </c>
     </row>
@@ -3377,12 +3885,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -3392,12 +3900,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -3407,12 +3915,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3422,12 +3930,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3437,12 +3945,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3452,12 +3960,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
         </is>
       </c>
     </row>
@@ -3467,12 +3975,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -3482,12 +3990,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba', 'Tsultrim Gyalwa'}</t>
         </is>
       </c>
     </row>
@@ -3497,12 +4005,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -3512,12 +4020,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P2614</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'Nyen Lotsawa Darma Drak'}</t>
         </is>
       </c>
     </row>
@@ -3527,12 +4035,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P8212</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'Devendrarakṣita'}</t>
         </is>
       </c>
     </row>
@@ -3542,12 +4050,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P1242</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'Géwai Lodrö'}</t>
         </is>
       </c>
     </row>
@@ -3557,12 +4065,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:zhang-yesh-d-', 'eft:ye-shes-sde', 'eft:yesh-d-', 'eft:band-yesh-d-', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -3572,12 +4080,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -3587,12 +4095,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:munivarma', 'eft:munivarman'}</t>
         </is>
       </c>
     </row>
@@ -3602,12 +4110,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -3617,12 +4125,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P2557</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
+          <t>{"'brom", "'brom rgyal ba'i 'byung gnas"}</t>
         </is>
       </c>
     </row>
@@ -3632,12 +4140,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:munivarma', 'eft:munivarman'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -3647,12 +4155,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'vajrvisramitra', 'eft:sakyasena', 'Sherap Ö'}</t>
         </is>
       </c>
     </row>
@@ -3662,12 +4170,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -3677,12 +4185,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -3692,12 +4200,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -3707,12 +4215,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
         </is>
       </c>
     </row>
@@ -3722,12 +4230,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P8271</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'Kumārarakṣita'}</t>
         </is>
       </c>
     </row>
@@ -3737,12 +4245,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3752,12 +4260,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:t-jnanagarbha', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -3767,12 +4275,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'Rinchen Zangpo', 'eft:rin-chen-bzang-po', 'rin chen bzag po'}</t>
         </is>
       </c>
     </row>
@@ -3782,12 +4290,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P4256</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'Lotsāwa Zangkyong (bzang skyong)'}</t>
         </is>
       </c>
     </row>
@@ -3797,12 +4305,297 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:danasila'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>P8273</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>P0TMPT007</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>P8280</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>{'subhasita'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>P8216</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>{'Śākya Lodrö'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>P3458</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>{'Gö Lhetsé'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>{'eft:siladharma'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>P8211</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>{'eft:vidyakaraprabha', 'bidyakaraprabha'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>P8228</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>{'eft:surendrabodhi'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>P8263</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>{'eft:leki-d-'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>P00KG07267</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>P1KG8854</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>{'eft:surendrabodhi', 'eft:silendrabodhi', 'eft:srilendrabodhi'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>P1321</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>{'Shang Buchikpa'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>P0TMP098</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>{'eft:jinavara'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>P8249</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>{'eft:dharmakara', 'Paṇḍita Dharmākara'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>P2551</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>{'blo ldan shes rab'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>P2956</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>{'eft:krsnapandita'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>P6453</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>{'Tsultrim Gyaltsen'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>P8171</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>{'eft:dharmasribhadra'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>P4255</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>{'eft:yesh-nyingpo', 'eft:ye-shes-snying-po', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
change handling of hyphenated numbers
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H124"/>
+  <dimension ref="A1:H123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,12 +477,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>eft:sarvajnadeva</t>
+          <t>eft:jinamitra-k-</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -497,12 +497,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>eft:vidyakaraprabha</t>
+          <t>eft:klu-i-rgyal-mtshan</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -517,12 +517,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>eft:dharmakara</t>
+          <t>eft:dzi-na-mi-tra-k-</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -537,12 +537,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>eft:jinamitra-k-</t>
+          <t>eft:cog-ro-klu-i-rgyal-mtshan</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -557,12 +557,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>eft:klu-i-rgyal-mtshan</t>
+          <t>eft:dharmakara</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -577,12 +577,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>eft:dzi-na-mi-tra-k-</t>
+          <t>eft:ban-de-dpal-gyi-lhun-po</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -597,12 +597,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>eft:cog-ro-klu-i-rgyal-mtshan</t>
+          <t>eft:ban-de-dpal-brtsegs</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -617,12 +617,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>eft:ban-de-dpal-gyi-lhun-po</t>
+          <t>eft:dpal-byor</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -637,12 +637,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>eft:ban-de-dpal-brtsegs</t>
+          <t>eft:surendrabodhi</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -657,12 +657,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>eft:dpal-byor</t>
+          <t>eft:jinamitra</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -677,12 +677,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>eft:surendrabodhi</t>
+          <t>eft:danasila</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -697,12 +697,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>eft:jinamitra</t>
+          <t>eft:munivarman</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -717,12 +717,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>eft:danasila</t>
+          <t>eft:prajnavarman</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -737,12 +737,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>eft:munivarman</t>
+          <t>eft:dpal-dbyangs</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -757,12 +757,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>eft:prajnavarman</t>
+          <t>eft:ska-ba-dpal-brtsegs</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -777,12 +777,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>eft:dpal-dbyangs</t>
+          <t>eft:silendrabodhi</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
@@ -797,12 +797,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>eft:ska-ba-dpal-brtsegs</t>
+          <t>eft:prajnavarma</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
@@ -817,12 +817,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>eft:silendrabodhi</t>
+          <t>eft:dipamkarasrijnana</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
@@ -837,12 +837,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>eft:prajnavarma</t>
+          <t>eft:buddhaprabha</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
@@ -857,12 +857,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>eft:dipamkarasrijnana</t>
+          <t>eft:ye-shes-sde</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
@@ -877,12 +877,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>eft:buddhaprabha</t>
+          <t>eft:dgon-gling-rma</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
@@ -897,12 +897,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>eft:ye-shes-sde</t>
+          <t>eft:dpal-gyi-lhun-po</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
@@ -917,12 +917,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>eft:dgon-gling-rma</t>
+          <t>eft:dpal-brtsegs</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
@@ -937,12 +937,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>eft:dpal-gyi-lhun-po</t>
+          <t>eft:sakyaprabha</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
@@ -957,12 +957,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>eft:dpal-brtsegs</t>
+          <t>eft:dharmatasila</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
@@ -977,12 +977,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>eft:sakyaprabha</t>
+          <t>eft:ye-shes-snying-po</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
@@ -997,12 +997,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>eft:dharmatasila</t>
+          <t>eft:visuddhasimha</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
@@ -1017,12 +1017,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>eft:ye-shes-snying-po</t>
+          <t>eft:dge-ba-dpal</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
@@ -1037,12 +1037,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>eft:visuddhasimha</t>
+          <t>eft:devacandra</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
@@ -1057,12 +1057,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>eft:dge-ba-dpal</t>
+          <t>eft:kamalagupta</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
@@ -1077,12 +1077,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>eft:devacandra</t>
+          <t>eft:rin-chen-bzang-po</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
@@ -1097,12 +1097,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>eft:kamalagupta</t>
+          <t>eft:rin-chen-tsho</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
@@ -1117,12 +1117,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>eft:rin-chen-bzang-po</t>
+          <t>eft:jnanagarbha</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
@@ -1137,12 +1137,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>eft:rin-chen-tsho</t>
+          <t>eft:sarvajnadeva</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
@@ -1157,12 +1157,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>eft:jnanagarbha</t>
+          <t>eft:vijayasila</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
@@ -1177,12 +1177,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>eft:vijayasila</t>
+          <t>eft:hwa-shang-zab-mo</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
@@ -1197,12 +1197,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>eft:hwa-shang-zab-mo</t>
+          <t>eft:rnam-par-mi-rtog-pa</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="D38" t="inlineStr"/>
@@ -1217,12 +1217,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>eft:rnam-par-mi-rtog-pa</t>
+          <t>eft:munivarma</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
@@ -1237,12 +1237,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>eft:munivarma</t>
+          <t>eft:ratnaraksita</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
@@ -1257,12 +1257,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>eft:ratnaraksita</t>
+          <t>eft:dharmasribhadra</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
@@ -1277,12 +1277,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>eft:dharmasribhadra</t>
+          <t>eft:gayadhara</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
@@ -1297,12 +1297,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>eft:gayadhara</t>
+          <t>eft:krsnapandita</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
@@ -1317,12 +1317,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>eft:krsnapandita</t>
+          <t>eft:tshul-khrims-rgyal-ba</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
@@ -1337,12 +1337,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>eft:tshul-khrims-rgyal-ba</t>
+          <t>eft:celu</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="D45" t="inlineStr"/>
@@ -1357,12 +1357,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>eft:celu</t>
+          <t>eft:jnanasiddhi</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="D46" t="inlineStr"/>
@@ -1377,12 +1377,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>eft:jnanasiddhi</t>
+          <t>eft:punyasambhava</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="D47" t="inlineStr"/>
@@ -1393,501 +1393,511 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>eft:punyasambhava</t>
+          <t>eft:palgyi-lh-npo</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr"/>
-      <c r="F48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>1-1</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Palgyi Lhünpo</t>
+        </is>
+      </c>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>eft:palgyi-lh-npo</t>
+          <t>eft:sarvanyadeva</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>1-1</t>
-        </is>
+      <c r="E49" t="n">
+        <v>5</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Palgyi Lhünpo</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr"/>
+          <t>sarvanyadeva</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>kha che'i mkhan po sarba dz+nyA de ba, 'mkhan po sarba dz+nyA de ba/', 'sarvajñādeva'</t>
+        </is>
+      </c>
       <c r="H49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>eft:sarvanyadeva</t>
+          <t>eft:vidyakaraprabha</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>sarvanyadeva</t>
+          <t>vidyakaraprabha</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>kha che'i mkhan po sarba dz+nyA de ba, 'mkhan po sarba dz+nyA de ba/', 'sarvajñādeva'</t>
+          <t>'rgya gar gyi mkhan po bid+yA ka ra pra b+ha', 'slob dpon bid+yA ka ra pra b+hA/', 'vidyākaraprabha'</t>
         </is>
       </c>
       <c r="H50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>eft:vidyakaraprabha</t>
+          <t>eft:jinamitra</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>vidyakaraprabha</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>'rgya gar gyi mkhan po bid+yA ka ra pra b+ha', 'slob dpon bid+yA ka ra pra b+hA/', 'vidyākaraprabha'</t>
-        </is>
-      </c>
+          <t>Jinamitra</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>eft:jinamitra</t>
+          <t>eft:sakyasena</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>?</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Jinamitra</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr"/>
+          <t>sakyasena</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>{'P8213': ['rgya gar gyi mkhan po bid+yA ka ra sing ha', 'slob dpon bIr+ya sing+ha pra b+ha/', 'vīryakarasiṁha,vīryasiṁha'], 'P8182': ['zhu chen gyi lots+tsha ba ban de dpal brtsegs', 'ska ba dpal brtsegs/']}</t>
+        </is>
+      </c>
       <c r="H52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>eft:sakyasena</t>
+          <t>eft:jnanasiddhi</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>sakyasena</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>{'P8213': ['rgya gar gyi mkhan po bid+yA ka ra sing ha', 'slob dpon bIr+ya sing+ha pra b+ha/', 'vīryakarasiṁha,vīryasiṁha'], 'P8182': ['zhu chen gyi lots+tsha ba ban de dpal brtsegs', 'ska ba dpal brtsegs/']}</t>
-        </is>
-      </c>
+          <t>jnanasiddhi</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>eft:jnanasiddhi</t>
+          <t>eft:anandasri-s-</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="n">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>jnanasiddhi</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr"/>
+          <t>anandasri (s)</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>paN+Di ta chen po A nan+da shrI', 'paN+Di ta A nan+da shrI', 'Ānandaśrī'</t>
+        </is>
+      </c>
       <c r="H54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>eft:anandasri-s-</t>
+          <t>eft:kawa-paltsek-under-the-name-paltsek-raksita-</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="n">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>anandasri (s)</t>
+          <t>Kawa Paltsek (under the name Paltsek Rakṣita)</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>paN+Di ta chen po A nan+da shrI', 'paN+Di ta A nan+da shrI', 'Ānandaśrī'</t>
+          <t>'zhu chen gyi lo tsa ba ban de dpal brtsegs rak+Shi ta', 'ska ba dpal brtsegs/'</t>
         </is>
       </c>
       <c r="H55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>eft:kawa-paltsek-under-the-name-paltsek-raksita-</t>
+          <t>eft:yesh-d-</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="n">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Kawa Paltsek (under the name Paltsek Rakṣita)</t>
+          <t>Yeshé Dé</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>'zhu chen gyi lo tsa ba ban de dpal brtsegs rak+Shi ta', 'ska ba dpal brtsegs/'</t>
+          <t>'zhu chen gyi lo ts+tsha ba ban de ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
         </is>
       </c>
       <c r="H56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>eft:yesh-d-</t>
+          <t>eft:danasila</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="n">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Yeshé Dé</t>
+          <t>Danaśila</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>'zhu chen gyi lo ts+tsha ba ban de ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
+          <t>'dA na shI la', 'paN chen dA na shI la/', 'dānaśīla'</t>
         </is>
       </c>
       <c r="H57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>eft:danasila</t>
+          <t>eft:t-vidyakarasimha</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="n">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Danaśila</t>
+          <t>t. Vidyākarasiṃha</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>'dA na shI la', 'paN chen dA na shI la/', 'dānaśīla'</t>
+          <t>'rgya gar gyi mkhan po bid+yA ka ra sing ha', 'slob dpon bIr+ya sing+ha pra b+ha/', 'vīryakarasiṁha,vīryasiṁha'</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>eft:t-vidyakarasimha</t>
+          <t>eft:yesh-nyingpo</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>t. Vidyākarasiṃha</t>
+          <t>Yeshé Nyingpo</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>'rgya gar gyi mkhan po bid+yA ka ra sing ha', 'slob dpon bIr+ya sing+ha pra b+ha/', 'vīryakarasiṁha,vīryasiṁha'</t>
+          <t>'lots+tsha ba ban de ye shes snying po', 'lo tsA ba ye shes snying po/', 'Jñānagarbha'</t>
         </is>
       </c>
       <c r="H59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>eft:yesh-nyingpo</t>
+          <t>eft:band-yesh-d-</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Yeshé Nyingpo</t>
+          <t>Bandé Yeshé Dé</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>'lots+tsha ba ban de ye shes snying po', 'lo tsA ba ye shes snying po/', 'Jñānagarbha'</t>
+          <t>'zhu chen gyi lots+tsha ba ban de ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
         </is>
       </c>
       <c r="H60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>eft:band-yesh-d-</t>
+          <t>eft:leki-d-</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="n">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Bandé Yeshé Dé</t>
+          <t>Leki Dé</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>'zhu chen gyi lots+tsha ba ban de ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
+          <t>'lo ts+tsha ba ban de legs kyi sde', 'legs kyi sde/'</t>
         </is>
       </c>
       <c r="H61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>eft:leki-d-</t>
+          <t>eft:surendrabodhi</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="n">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Leki Dé</t>
+          <t>Surendrabodhi</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>'lo ts+tsha ba ban de legs kyi sde', 'legs kyi sde/'</t>
+          <t>'shI len dra bo d+hi', 'shI len+dra bo d+hi/', 'śīlendrabodhi'</t>
         </is>
       </c>
       <c r="H62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>eft:surendrabodhi</t>
+          <t>eft:yesh-d-ye-shes-sde-</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Surendrabodhi</t>
+          <t>Yeshé Dé (ye shes sde)</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>'shI len dra bo d+hi', 'shI len+dra bo d+hi/', 'śīlendrabodhi'</t>
+          <t>'zhu chen gyi lo tsA ba _ban de ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
         </is>
       </c>
       <c r="H63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>eft:yesh-d-ye-shes-sde-</t>
+          <t>eft:srilendrabodhi</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="n">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Yeshé Dé (ye shes sde)</t>
+          <t>Śrīlendrabodhi</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>'zhu chen gyi lo tsA ba _ban de ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
+          <t>'rgya gar gyi mkhan po shI len dra bo d+hi', 'shI len+dra bo d+hi/', 'śīlendrabodhi'</t>
         </is>
       </c>
       <c r="H64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>eft:srilendrabodhi</t>
+          <t>eft:silendrabodhi</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1897,139 +1907,135 @@
       </c>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="n">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Śrīlendrabodhi</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>'rgya gar gyi mkhan po shI len dra bo d+hi', 'shI len+dra bo d+hi/', 'śīlendrabodhi'</t>
-        </is>
-      </c>
+          <t>Śilendrabodhi</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>eft:silendrabodhi</t>
+          <t>eft:dipamkarasrijnana</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="n">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Śilendrabodhi</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr"/>
+          <t>Dīpaṃkaraśrījñāna</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>'rgya gar gyi mkhan po dI paM ka ra shrI dz+nyA na', 'slob dpon mar med mdzad bzang po/', 'dīpaṁkaraśrijñāna,atīśa'</t>
+        </is>
+      </c>
       <c r="H66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>eft:dipamkarasrijnana</t>
+          <t>eft:prajnavarma</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="n">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Dīpaṃkaraśrījñāna</t>
+          <t>prajnavarma</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>'rgya gar gyi mkhan po dI paM ka ra shrI dz+nyA na', 'slob dpon mar med mdzad bzang po/', 'dīpaṁkaraśrijñāna,atīśa'</t>
+          <t>'pradz+nyA bad+ma', 'slob dpon shes rab go cha/', 'prajñāvarman'</t>
         </is>
       </c>
       <c r="H67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>eft:prajnavarma</t>
+          <t>eft:dharmapala</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="n">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>prajnavarma</t>
+          <t>Dharmapāla</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>'pradz+nyA bad+ma', 'slob dpon shes rab go cha/', 'prajñāvarman'</t>
+          <t>'d+harma pA la', 'dpal ldan chos skyong /'</t>
         </is>
       </c>
       <c r="H68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>eft:dharmapala</t>
+          <t>eft:t-jnanagarbha</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="n">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Dharmapāla</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>'d+harma pA la', 'dpal ldan chos skyong /'</t>
-        </is>
-      </c>
+          <t>t. Jñānagarbha</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -2038,7 +2044,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="D70" t="inlineStr"/>
@@ -2050,76 +2056,80 @@
           <t>t. Jñānagarbha</t>
         </is>
       </c>
-      <c r="G70" t="inlineStr"/>
-      <c r="H70" t="inlineStr"/>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>{'P8217': ['rgya gar gyi mkhan po dz+nyA na gar b+ha', 'dz+nyA na gar b+ha/', 'jñānagarbha ?'], 'P4255': ['lots+tsha ba ban+de ye shes snying po', 'lo tsA ba ye shes snying po/', 'Jñānagarbha']</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Note: this is ambiguous. I wonder if the BDRC entries refer to different people (one is Sanskrit, the other is Tibetan, but they translate to each other)</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>eft:t-jnanagarbha</t>
+          <t>eft:vidyakarasimha</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="n">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>t. Jñānagarbha</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>{'P8217': ['rgya gar gyi mkhan po dz+nyA na gar b+ha', 'dz+nyA na gar b+ha/', 'jñānagarbha ?'], 'P4255': ['lots+tsha ba ban+de ye shes snying po', 'lo tsA ba ye shes snying po/', 'Jñānagarbha']</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>Note: this is ambiguous. I wonder if the BDRC entries refer to different people (one is Sanskrit, the other is Tibetan, but they translate to each other)</t>
-        </is>
-      </c>
+          <t>Vidyākarasiṃha</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>eft:vidyakarasimha</t>
+          <t>eft:dharmatasila</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="n">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Vidyākarasiṃha</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr"/>
+          <t>Dharmatāśila</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>'zhu chen gyi lots+tsha ba ban de d+harma tA shI la', 'zhu chen gyi lo tsA ba dharma tA shI la/', 'Dharmatāśīla'</t>
+        </is>
+      </c>
       <c r="H72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>eft:dharmatasila</t>
+          <t>eft:ch-nyi-tsultrim</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2129,549 +2139,543 @@
       </c>
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="n">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Dharmatāśila</t>
+          <t>Chönyi Tsultrim</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>'zhu chen gyi lots+tsha ba ban de d+harma tA shI la', 'zhu chen gyi lo tsA ba dharma tA shI la/', 'Dharmatāśīla'</t>
+          <t xml:space="preserve"> 'lo ts+tsha ba ban de chos nyid tshul khrims', 'zhu chen gyi lo tsA ba dharma tA shI la/', 'Dharmatāśīla'</t>
         </is>
       </c>
       <c r="H73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>eft:ch-nyi-tsultrim</t>
+          <t>eft:jnanasidhi</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="n">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Chönyi Tsultrim</t>
+          <t>jnanasidhi</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'lo ts+tsha ba ban de chos nyid tshul khrims', 'zhu chen gyi lo tsA ba dharma tA shI la/', 'Dharmatāśīla'</t>
+          <t>'dz+nyA na sid+d+hi', 'dz+nyA na sid+dhi/', 'jñānasiddhi'</t>
         </is>
       </c>
       <c r="H74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>eft:jnanasidhi</t>
+          <t>eft:paltsek</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="n">
-        <v>178</v>
+        <v>225</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>jnanasidhi</t>
+          <t>Paltsek</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>'dz+nyA na sid+d+hi', 'dz+nyA na sid+dhi/', 'jñānasiddhi'</t>
+          <t>'zhu chen gyi lo ts+tsha ba ban de dpal brtsegs', 'ska ba dpal brtsegs/'</t>
         </is>
       </c>
       <c r="H75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>eft:paltsek</t>
+          <t>eft:rinchen-tso</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="n">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Paltsek</t>
+          <t>Rinchen Tso</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>'zhu chen gyi lo ts+tsha ba ban de dpal brtsegs', 'ska ba dpal brtsegs/'</t>
+          <t>lo ts+tsha ba ban de rin chen 'tsho, "lo tsA ba rin chen 'tsho/"</t>
         </is>
       </c>
       <c r="H76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>eft:rinchen-tso</t>
+          <t>eft:manjusrigarbha</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="n">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Rinchen Tso</t>
+          <t>Mañjuśrīgarbha</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>lo ts+tsha ba ban de rin chen 'tsho, "lo tsA ba rin chen 'tsho/"</t>
+          <t>'rgya gar gyi mkhan po many+dzu shrI gar+b+ha', 'mkhan po many+dzu shrI gar+b+ha/', 'majuśrīgarbha'</t>
         </is>
       </c>
       <c r="H77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>eft:manjusrigarbha</t>
+          <t>eft:siladharma</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="n">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Mañjuśrīgarbha</t>
+          <t>siladharma</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>'rgya gar gyi mkhan po many+dzu shrI gar+b+ha', 'mkhan po many+dzu shrI gar+b+ha/', 'majuśrīgarbha'</t>
+          <t>{'P0TMPT007': ["rgya gar gyi d+harma rgya'i yi ge las ban de rnam par mi rtog", 'rnam par mi rtog pa']}</t>
         </is>
       </c>
       <c r="H78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>eft:siladharma</t>
+          <t>eft:zhang-yesh-d-</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="n">
-        <v>242</v>
+        <v>309</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>siladharma</t>
+          <t>Zhang Yeshé Dé</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>{'P0TMPT007': ["rgya gar gyi d+harma rgya'i yi ge las ban de rnam par mi rtog", 'rnam par mi rtog pa']}</t>
+          <t>zhu chen gyi lo ts+tsha ba ban de zhang ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
         </is>
       </c>
       <c r="H79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>eft:zhang-yesh-d-</t>
+          <t>eft:sherab-lekpa</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="n">
-        <v>309</v>
+        <v>349</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Zhang Yeshé Dé</t>
+          <t>Sherab Lekpa</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>zhu chen gyi lo ts+tsha ba ban de zhang ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
+          <t>'zhu chen gyi lots+tsha ba dge slong shes rab legs pa', 'shes rab legs pa/'</t>
         </is>
       </c>
       <c r="H80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>eft:sherab-lekpa</t>
+          <t>eft:sakya-yesh-</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="n">
-        <v>349</v>
+        <v>384</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Sherab Lekpa</t>
+          <t>Śākya Yeshé</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>'zhu chen gyi lots+tsha ba dge slong shes rab legs pa', 'shes rab legs pa/'</t>
+          <t>'lots+tsha ba dge slong shAkya ye shes', 'brog mi lo tsA ba shAkya ye shes/'</t>
         </is>
       </c>
       <c r="H81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>eft:sakya-yesh-</t>
+          <t>eft:jinavara</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="n">
-        <v>384</v>
+        <v>425</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Śākya Yeshé</t>
+          <t>Jinavara</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>'lots+tsha ba dge slong shAkya ye shes', 'brog mi lo tsA ba shAkya ye shes/'</t>
+          <t>'rgya gar gyi mkhan po dzi na bar', 'rgya gar gyi mkhan po dzi na bar', 'Jinapara'</t>
         </is>
       </c>
       <c r="H82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>eft:jinavara</t>
+          <t>eft:trakpa-gyaltsen</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="n">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Jinavara</t>
+          <t>Trakpa Gyaltsen</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>'rgya gar gyi mkhan po dzi na bar', 'rgya gar gyi mkhan po dzi na bar', 'Jinapara'</t>
+          <t>'lo ts+tsha ba grags pa rgyal mtshan', 'yar lung lo tsA ba grags pa rgyal mtshan/'</t>
         </is>
       </c>
       <c r="H83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>eft:trakpa-gyaltsen</t>
+          <t>eft:phakpa-sherab</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="n">
-        <v>431</v>
+        <v>498</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Trakpa Gyaltsen</t>
+          <t>Phakpa Sherab</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>'lo ts+tsha ba grags pa rgyal mtshan', 'yar lung lo tsA ba grags pa rgyal mtshan/'</t>
+          <t>bod kyi lo ts+tsha ba 'phags pa shes rab, "zangs dkar lo tsA ba 'phags pa shes rab/"</t>
         </is>
       </c>
       <c r="H84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>eft:phakpa-sherab</t>
+          <t>eft:kumarakalasa</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="n">
-        <v>498</v>
+        <v>543</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Phakpa Sherab</t>
+          <t>Kumārakalaśa</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>bod kyi lo ts+tsha ba 'phags pa shes rab, "zangs dkar lo tsA ba 'phags pa shes rab/"</t>
+          <t>'rgya gar gyi mkhan po dge bsnyen chen po ku mA ra ka la sha', 'mkhan po gzhon nu bum pa/', 'kumārakalasa'</t>
         </is>
       </c>
       <c r="H85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>eft:kumarakalasa</t>
+          <t>eft:dipamkara-srijnana</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="n">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Kumārakalaśa</t>
+          <t>Dīpaṃkara Śrījñāna</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>'rgya gar gyi mkhan po dge bsnyen chen po ku mA ra ka la sha', 'mkhan po gzhon nu bum pa/', 'kumārakalasa'</t>
+          <t>rgya gar gyi mkhan po chen po dI paM ka ra shrIdz+nyA na', 'slob dpon mar med mdzad bzang po/', 'dīpaṁkaraśrijñāna,atīśa'</t>
         </is>
       </c>
       <c r="H86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>eft:dipamkara-srijnana</t>
+          <t>eft:pa-tshab-nyi-ma-grags</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="D87" t="inlineStr"/>
       <c r="E87" t="n">
-        <v>544</v>
+        <v>850</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Dīpaṃkara Śrījñāna</t>
+          <t>pa tshab nyi ma grags</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>rgya gar gyi mkhan po chen po dI paM ka ra shrIdz+nyA na', 'slob dpon mar med mdzad bzang po/', 'dīpaṁkaraśrijñāna,atīśa'</t>
+          <t>'lo ts+tsha ba pa tsha ba nyi ma grags', 'pa tshab lo tsA ba nyi ma grags pa/'</t>
         </is>
       </c>
       <c r="H87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>eft:pa-tshab-nyi-ma-grags</t>
+          <t>eft:band-yesh-de</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="n">
-        <v>850</v>
+        <v>725</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>pa tshab nyi ma grags</t>
+          <t>Bandé Yeshé De</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>'lo ts+tsha ba pa tsha ba nyi ma grags', 'pa tshab lo tsA ba nyi ma grags pa/'</t>
+          <t>'zhu chen gyi lots+tsha ba ban+de ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
         </is>
       </c>
       <c r="H88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>eft:band-yesh-de</t>
+          <t>eft:buddhakaravarma</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="D89" t="inlineStr"/>
       <c r="E89" t="n">
-        <v>725</v>
+        <v>747</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Bandé Yeshé De</t>
+          <t>Buddhākaravarma</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>'zhu chen gyi lots+tsha ba ban+de ye shes sde', 'sna nam btsun pa ye shes sde/'</t>
+          <t xml:space="preserve">'rgya gar gyi mkhan po bud+d+ha A ka ra ba rma', 'bud d+ha ka ra wa rman/', 'buddhakaravarman ?' </t>
         </is>
       </c>
       <c r="H89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>eft:buddhakaravarma</t>
+          <t>eft:g-ch-drup</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P8221</t>
         </is>
       </c>
       <c r="D90" t="inlineStr"/>
-      <c r="E90" t="n">
-        <v>747</v>
-      </c>
+      <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Buddhākaravarma</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t xml:space="preserve">'rgya gar gyi mkhan po bud+d+ha A ka ra ba rma', 'bud d+ha ka ra wa rman/', 'buddhakaravarman ?' </t>
-        </is>
-      </c>
+          <t>Gö Chödrup</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>eft:g-ch-drup</t>
+          <t>eft:wang-phab-zhwun-wang-phan-zhun-</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>P8221</t>
+          <t>P8276</t>
         </is>
       </c>
       <c r="D91" t="inlineStr"/>
       <c r="E91" t="inlineStr"/>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Gö Chödrup</t>
+          <t>wang phab zhwun (wang phan zhun)</t>
         </is>
       </c>
       <c r="G91" t="inlineStr"/>
@@ -2679,23 +2683,23 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>eft:wang-phab-zhwun-wang-phan-zhun-</t>
+          <t>eft:dge-ba-i-blo-gros</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>P8276</t>
+          <t>P8278</t>
         </is>
       </c>
       <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr"/>
       <c r="F92" t="inlineStr">
         <is>
-          <t>wang phab zhwun (wang phan zhun)</t>
+          <t>dge ba'i blo gros</t>
         </is>
       </c>
       <c r="G92" t="inlineStr"/>
@@ -2703,23 +2707,23 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>eft:dge-ba-i-blo-gros</t>
+          <t>eft:rgya-mtsho-i-sde</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>P8278</t>
+          <t>P8277</t>
         </is>
       </c>
       <c r="D93" t="inlineStr"/>
       <c r="E93" t="inlineStr"/>
       <c r="F93" t="inlineStr">
         <is>
-          <t>dge ba'i blo gros</t>
+          <t>rgya mtsho'i sde</t>
         </is>
       </c>
       <c r="G93" t="inlineStr"/>
@@ -2727,23 +2731,23 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>eft:rgya-mtsho-i-sde</t>
+          <t>eft:th-nmi-sambhota</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>P8277</t>
+          <t>P5788</t>
         </is>
       </c>
       <c r="D94" t="inlineStr"/>
       <c r="E94" t="inlineStr"/>
       <c r="F94" t="inlineStr">
         <is>
-          <t>rgya mtsho'i sde</t>
+          <t>Thönmi Sambhoṭa</t>
         </is>
       </c>
       <c r="G94" t="inlineStr"/>
@@ -2751,23 +2755,23 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>eft:th-nmi-sambhota</t>
+          <t>eft:tsultrim-gyaltsen</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>P5788</t>
+          <t>P6453</t>
         </is>
       </c>
       <c r="D95" t="inlineStr"/>
       <c r="E95" t="inlineStr"/>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Thönmi Sambhoṭa</t>
+          <t>Tsultrim Gyaltsen</t>
         </is>
       </c>
       <c r="G95" t="inlineStr"/>
@@ -2775,23 +2779,23 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>eft:tsultrim-gyaltsen</t>
+          <t>eft:shang-buchikpa</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>P6453</t>
+          <t>P1321</t>
         </is>
       </c>
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr"/>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Tsultrim Gyaltsen</t>
+          <t>Shang Buchikpa</t>
         </is>
       </c>
       <c r="G96" t="inlineStr"/>
@@ -2799,23 +2803,23 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>eft:shang-buchikpa</t>
+          <t>eft:sherap-</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>P1321</t>
+          <t>?</t>
         </is>
       </c>
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="inlineStr"/>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Shang Buchikpa</t>
+          <t>Sherap Ö</t>
         </is>
       </c>
       <c r="G97" t="inlineStr"/>
@@ -2823,23 +2827,23 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>eft:sherap-</t>
+          <t>eft:pandita-dharmakara</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr"/>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Sherap Ö</t>
+          <t>Paṇḍita Dharmākara</t>
         </is>
       </c>
       <c r="G98" t="inlineStr"/>
@@ -2847,23 +2851,23 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>eft:pandita-dharmakara</t>
+          <t>eft:lotsawa-zangkyong-bzang-skyong-</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P4256</t>
         </is>
       </c>
       <c r="D99" t="inlineStr"/>
       <c r="E99" t="inlineStr"/>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Paṇḍita Dharmākara</t>
+          <t>Lotsāwa Zangkyong (bzang skyong)</t>
         </is>
       </c>
       <c r="G99" t="inlineStr"/>
@@ -2871,23 +2875,23 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>eft:lotsawa-zangkyong-bzang-skyong-</t>
+          <t>eft:nyen-lotsawa-darma-drak</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>P4256</t>
+          <t>P2614</t>
         </is>
       </c>
       <c r="D100" t="inlineStr"/>
       <c r="E100" t="inlineStr"/>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Lotsāwa Zangkyong (bzang skyong)</t>
+          <t>Nyen Lotsawa Darma Drak</t>
         </is>
       </c>
       <c r="G100" t="inlineStr"/>
@@ -2895,23 +2899,23 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>eft:nyen-lotsawa-darma-drak</t>
+          <t>eft:patsap-nyima-drak-</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>P2614</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="D101" t="inlineStr"/>
       <c r="E101" t="inlineStr"/>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Nyen Lotsawa Darma Drak</t>
+          <t>Patsap Nyima Drak [?]</t>
         </is>
       </c>
       <c r="G101" t="inlineStr"/>
@@ -2919,23 +2923,23 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>eft:patsap-nyima-drak-</t>
+          <t>eft:vajrvisramitra</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>?</t>
         </is>
       </c>
       <c r="D102" t="inlineStr"/>
       <c r="E102" t="inlineStr"/>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Patsap Nyima Drak [?]</t>
+          <t>vajrvisramitra</t>
         </is>
       </c>
       <c r="G102" t="inlineStr"/>
@@ -2943,23 +2947,23 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>eft:vajrvisramitra</t>
+          <t>eft:bidyakaraprabha</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="D103" t="inlineStr"/>
       <c r="E103" t="inlineStr"/>
       <c r="F103" t="inlineStr">
         <is>
-          <t>vajrvisramitra</t>
+          <t>bidyakaraprabha</t>
         </is>
       </c>
       <c r="G103" t="inlineStr"/>
@@ -2967,23 +2971,23 @@
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>eft:bidyakaraprabha</t>
+          <t>eft:subhasita</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P8280</t>
         </is>
       </c>
       <c r="D104" t="inlineStr"/>
       <c r="E104" t="inlineStr"/>
       <c r="F104" t="inlineStr">
         <is>
-          <t>bidyakaraprabha</t>
+          <t>subhasita</t>
         </is>
       </c>
       <c r="G104" t="inlineStr"/>
@@ -2991,23 +2995,23 @@
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>eft:subhasita</t>
+          <t>eft:rin-chen-bzag-po</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>P8280</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="D105" t="inlineStr"/>
       <c r="E105" t="inlineStr"/>
       <c r="F105" t="inlineStr">
         <is>
-          <t>subhasita</t>
+          <t>rin chen bzag po</t>
         </is>
       </c>
       <c r="G105" t="inlineStr"/>
@@ -3015,23 +3019,23 @@
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>eft:rin-chen-bzag-po</t>
+          <t>eft:-brom-rgyal-ba-i-byung-gnas</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P2557</t>
         </is>
       </c>
       <c r="D106" t="inlineStr"/>
       <c r="E106" t="inlineStr"/>
       <c r="F106" t="inlineStr">
         <is>
-          <t>rin chen bzag po</t>
+          <t>'brom rgyal ba'i 'byung gnas</t>
         </is>
       </c>
       <c r="G106" t="inlineStr"/>
@@ -3039,11 +3043,11 @@
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>eft:-brom-rgyal-ba-i-byung-gnas</t>
+          <t>eft:-brom</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3055,7 +3059,7 @@
       <c r="E107" t="inlineStr"/>
       <c r="F107" t="inlineStr">
         <is>
-          <t>'brom rgyal ba'i 'byung gnas</t>
+          <t>'brom</t>
         </is>
       </c>
       <c r="G107" t="inlineStr"/>
@@ -3063,23 +3067,23 @@
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>eft:-brom</t>
+          <t>eft:blo-ldan-shes-rab</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>P2557</t>
+          <t>P2551</t>
         </is>
       </c>
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr"/>
       <c r="F108" t="inlineStr">
         <is>
-          <t>'brom</t>
+          <t>blo ldan shes rab</t>
         </is>
       </c>
       <c r="G108" t="inlineStr"/>
@@ -3087,23 +3091,23 @@
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>eft:blo-ldan-shes-rab</t>
+          <t>eft:yesh-de</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>P2551</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr"/>
       <c r="F109" t="inlineStr">
         <is>
-          <t>blo ldan shes rab</t>
+          <t>Yeshé De</t>
         </is>
       </c>
       <c r="G109" t="inlineStr"/>
@@ -3111,23 +3115,23 @@
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>eft:yesh-de</t>
+          <t>eft:lotsawa-band-dharmatasila</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="D110" t="inlineStr"/>
       <c r="E110" t="inlineStr"/>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Yeshé De</t>
+          <t>Lotsawa Bandé Dharmatāśīla</t>
         </is>
       </c>
       <c r="G110" t="inlineStr"/>
@@ -3135,23 +3139,23 @@
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>eft:lotsawa-band-dharmatasila</t>
+          <t>eft:gewai-lodr-</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P8278</t>
         </is>
       </c>
       <c r="D111" t="inlineStr"/>
       <c r="E111" t="inlineStr"/>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Lotsawa Bandé Dharmatāśīla</t>
+          <t>Gewai Lodrö</t>
         </is>
       </c>
       <c r="G111" t="inlineStr"/>
@@ -3159,23 +3163,23 @@
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>eft:gewai-lodr-</t>
+          <t>eft:devendraraksita</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>P8278</t>
+          <t>P8212</t>
         </is>
       </c>
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="inlineStr"/>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Gewai Lodrö</t>
+          <t>Devendrarakṣita</t>
         </is>
       </c>
       <c r="G112" t="inlineStr"/>
@@ -3183,23 +3187,23 @@
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>eft:devendraraksita</t>
+          <t>eft:kumararaksita</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>P8212</t>
+          <t>P8271</t>
         </is>
       </c>
       <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr"/>
       <c r="F113" t="inlineStr">
         <is>
-          <t>Devendrarakṣita</t>
+          <t>Kumārarakṣita</t>
         </is>
       </c>
       <c r="G113" t="inlineStr"/>
@@ -3207,23 +3211,23 @@
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>eft:kumararaksita</t>
+          <t>eft:gew-pal</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>P8271</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="D114" t="inlineStr"/>
       <c r="E114" t="inlineStr"/>
       <c r="F114" t="inlineStr">
         <is>
-          <t>Kumārarakṣita</t>
+          <t>Gewé Pal</t>
         </is>
       </c>
       <c r="G114" t="inlineStr"/>
@@ -3231,23 +3235,23 @@
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>eft:gew-pal</t>
+          <t>eft:band-paltsek</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr"/>
       <c r="F115" t="inlineStr">
         <is>
-          <t>Gewé Pal</t>
+          <t>Bandé Paltsek</t>
         </is>
       </c>
       <c r="G115" t="inlineStr"/>
@@ -3255,23 +3259,23 @@
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>eft:band-paltsek</t>
+          <t>eft:rinchen-zangpo</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr"/>
       <c r="F116" t="inlineStr">
         <is>
-          <t>Bandé Paltsek</t>
+          <t>Rinchen Zangpo</t>
         </is>
       </c>
       <c r="G116" t="inlineStr"/>
@@ -3279,23 +3283,23 @@
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>eft:rinchen-zangpo</t>
+          <t>eft:g-lhets-</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P3458</t>
         </is>
       </c>
       <c r="D117" t="inlineStr"/>
       <c r="E117" t="inlineStr"/>
       <c r="F117" t="inlineStr">
         <is>
-          <t>Rinchen Zangpo</t>
+          <t>Gö Lhetsé</t>
         </is>
       </c>
       <c r="G117" t="inlineStr"/>
@@ -3303,23 +3307,23 @@
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>eft:g-lhets-</t>
+          <t>eft:sakya-lodr-</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>P3458</t>
+          <t>P8216</t>
         </is>
       </c>
       <c r="D118" t="inlineStr"/>
       <c r="E118" t="inlineStr"/>
       <c r="F118" t="inlineStr">
         <is>
-          <t>Gö Lhetsé</t>
+          <t>Śākya Lodrö</t>
         </is>
       </c>
       <c r="G118" t="inlineStr"/>
@@ -3327,23 +3331,23 @@
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>eft:sakya-lodr-</t>
+          <t>eft:g-wai-lodr-</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>P8216</t>
+          <t>P1242</t>
         </is>
       </c>
       <c r="D119" t="inlineStr"/>
       <c r="E119" t="inlineStr"/>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Śākya Lodrö</t>
+          <t>Géwai Lodrö</t>
         </is>
       </c>
       <c r="G119" t="inlineStr"/>
@@ -3351,23 +3355,23 @@
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>eft:g-wai-lodr-</t>
+          <t>eft:tsultrim-gyalwa</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>P1242</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr"/>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Géwai Lodrö</t>
+          <t>Tsultrim Gyalwa</t>
         </is>
       </c>
       <c r="G120" t="inlineStr"/>
@@ -3375,23 +3379,23 @@
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>eft:tsultrim-gyalwa</t>
+          <t>eft:patsap-nyima-drak-</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="D121" t="inlineStr"/>
       <c r="E121" t="inlineStr"/>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Tsultrim Gyalwa</t>
+          <t>Patsap Nyima Drak [?]</t>
         </is>
       </c>
       <c r="G121" t="inlineStr"/>
@@ -3399,23 +3403,23 @@
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>eft:patsap-nyima-drak-</t>
+          <t>eft:ch-kyi-sherab</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P3890</t>
         </is>
       </c>
       <c r="D122" t="inlineStr"/>
       <c r="E122" t="inlineStr"/>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Patsap Nyima Drak [?]</t>
+          <t>Chökyi Sherab</t>
         </is>
       </c>
       <c r="G122" t="inlineStr"/>
@@ -3423,51 +3427,27 @@
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>eft:ch-kyi-sherab</t>
+          <t>eft:vairocanaraksita</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>P3890</t>
+          <t>P4CZ15308</t>
         </is>
       </c>
       <c r="D123" t="inlineStr"/>
       <c r="E123" t="inlineStr"/>
       <c r="F123" t="inlineStr">
         <is>
-          <t>Chökyi Sherab</t>
+          <t>vairocanaraksita</t>
         </is>
       </c>
       <c r="G123" t="inlineStr"/>
       <c r="H123" t="inlineStr"/>
-    </row>
-    <row r="124">
-      <c r="A124" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>eft:vairocanaraksita</t>
-        </is>
-      </c>
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>P4CZ15308</t>
-        </is>
-      </c>
-      <c r="D124" t="inlineStr"/>
-      <c r="E124" t="inlineStr"/>
-      <c r="F124" t="inlineStr">
-        <is>
-          <t>vairocanaraksita</t>
-        </is>
-      </c>
-      <c r="G124" t="inlineStr"/>
-      <c r="H124" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3506,12 +3486,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs', 'eft:band-paltsek', 'eft:ban-de-dpal-brtsegs', 'eft:dpal-brtsegs'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -3521,12 +3501,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -3536,12 +3516,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P8212</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:devendraraksita'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -3551,12 +3531,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
         </is>
       </c>
     </row>
@@ -3566,12 +3546,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:bidyakaraprabha', 'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -3581,12 +3561,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P1242</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags', 'eft:patsap-nyima-drak-'}</t>
+          <t>{'eft:g-wai-lodr-'}</t>
         </is>
       </c>
     </row>
@@ -3596,12 +3576,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P2614</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:nyen-lotsawa-darma-drak'}</t>
+          <t>{'eft:dge-ba-dpal', 'eft:gew-pal'}</t>
         </is>
       </c>
     </row>
@@ -3611,12 +3591,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P8221</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:g-ch-drup'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -3626,12 +3606,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P8278</t>
+          <t>P8221</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:gewai-lodr-', 'eft:dge-ba-i-blo-gros'}</t>
+          <t>{'eft:g-ch-drup'}</t>
         </is>
       </c>
     </row>
@@ -3641,12 +3621,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
         </is>
       </c>
     </row>
@@ -3656,12 +3636,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -3671,12 +3651,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
+          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3686,12 +3666,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -3701,12 +3681,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -3716,12 +3696,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P2551</t>
+          <t>P2557</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:blo-ldan-shes-rab'}</t>
+          <t>{'eft:-brom-rgyal-ba-i-byung-gnas', 'eft:-brom'}</t>
         </is>
       </c>
     </row>
@@ -3731,12 +3711,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P4CZ15308</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:vairocanaraksita'}</t>
+          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3746,12 +3726,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P3890</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:ch-kyi-sherab'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
     </row>
@@ -3761,12 +3741,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P8276</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:wang-phab-zhwun-wang-phan-zhun-'}</t>
         </is>
       </c>
     </row>
@@ -3776,12 +3756,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:surendrabodhi', 'eft:srilendrabodhi'}</t>
+          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:band-paltsek', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:dpal-brtsegs'}</t>
         </is>
       </c>
     </row>
@@ -3791,12 +3771,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P8280</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:subhasita'}</t>
         </is>
       </c>
     </row>
@@ -3806,12 +3786,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:tshul-khrims-rgyal-ba', 'eft:tsultrim-gyalwa'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -3821,12 +3801,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:ch-nyi-tsultrim', 'eft:lotsawa-band-dharmatasila', 'eft:dharmatasila'}</t>
         </is>
       </c>
     </row>
@@ -3836,12 +3816,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -3851,12 +3831,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3866,12 +3846,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3881,12 +3861,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:yesh-nyingpo', 'eft:ye-shes-snying-po', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3911,12 +3891,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
         </is>
       </c>
     </row>
@@ -3926,12 +3906,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P3458</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'eft:g-lhets-'}</t>
         </is>
       </c>
     </row>
@@ -3941,12 +3921,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -3956,12 +3936,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -3971,12 +3951,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags', 'eft:patsap-nyima-drak-'}</t>
         </is>
       </c>
     </row>
@@ -3986,12 +3966,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P1242</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:g-wai-lodr-'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -4001,12 +3981,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P8216</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:sakya-lodr-'}</t>
         </is>
       </c>
     </row>
@@ -4016,12 +3996,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P8280</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:subhasita'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -4031,12 +4011,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:vajrvisramitra', 'eft:sherap-', 'eft:sakyasena'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
     </row>
@@ -4046,12 +4026,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
     </row>
@@ -4061,12 +4041,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P2614</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha', 'eft:bidyakaraprabha'}</t>
+          <t>{'eft:nyen-lotsawa-darma-drak'}</t>
         </is>
       </c>
     </row>
@@ -4076,12 +4056,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P4CZ15308</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:ye-shes-snying-po', 'eft:yesh-nyingpo', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:vairocanaraksita'}</t>
         </is>
       </c>
     </row>
@@ -4091,12 +4071,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P8278</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:gewai-lodr-', 'eft:dge-ba-i-blo-gros'}</t>
         </is>
       </c>
     </row>
@@ -4106,12 +4086,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:dharmakara', 'eft:pandita-dharmakara'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -4121,12 +4101,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P6453</t>
+          <t>P4256</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:tsultrim-gyaltsen'}</t>
+          <t>{'eft:lotsawa-zangkyong-bzang-skyong-'}</t>
         </is>
       </c>
     </row>
@@ -4136,12 +4116,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:vajrvisramitra', 'eft:sherap-', 'eft:sakyasena'}</t>
         </is>
       </c>
     </row>
@@ -4151,12 +4131,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P1321</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:shang-buchikpa'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -4166,12 +4146,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:vidyakarasimha', 'eft:t-vidyakarasimha'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -4181,12 +4161,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P2557</t>
+          <t>P8212</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:-brom-rgyal-ba-i-byung-gnas', 'eft:-brom'}</t>
+          <t>{'eft:devendraraksita'}</t>
         </is>
       </c>
     </row>
@@ -4196,12 +4176,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P8271</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
+          <t>{'eft:kumararaksita'}</t>
         </is>
       </c>
     </row>
@@ -4211,12 +4191,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -4226,12 +4206,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -4241,12 +4221,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P8276</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:wang-phab-zhwun-wang-phan-zhun-'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -4256,12 +4236,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:band-yesh-d-', 'eft:yesh-de', 'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
     </row>
@@ -4271,12 +4251,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P8271</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:kumararaksita'}</t>
+          <t>{'eft:srilendrabodhi', 'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -4286,12 +4266,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:lotsawa-band-dharmatasila', 'eft:dharmatasila'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -4301,12 +4281,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -4316,12 +4296,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P2551</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>{'eft:yesh-de', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-d-', 'eft:band-yesh-de', 'eft:zhang-yesh-d-', 'eft:yesh-d-'}</t>
+          <t>{'eft:blo-ldan-shes-rab'}</t>
         </is>
       </c>
     </row>
@@ -4331,12 +4311,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -4346,12 +4326,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>P8216</t>
+          <t>P5788</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>{'eft:sakya-lodr-'}</t>
+          <t>{'eft:th-nmi-sambhota'}</t>
         </is>
       </c>
     </row>
@@ -4361,12 +4341,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -4376,12 +4356,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal', 'eft:gew-pal'}</t>
+          <t>{'eft:pandita-dharmakara', 'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -4391,12 +4371,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -4406,12 +4386,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
     </row>
@@ -4421,12 +4401,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P1321</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:shang-buchikpa'}</t>
         </is>
       </c>
     </row>
@@ -4436,12 +4416,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -4451,12 +4431,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>P3458</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>{'eft:g-lhets-'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -4466,12 +4446,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -4481,12 +4461,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>P4256</t>
+          <t>P8277</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>{'eft:lotsawa-zangkyong-bzang-skyong-'}</t>
+          <t>{'eft:rgya-mtsho-i-sde'}</t>
         </is>
       </c>
     </row>
@@ -4496,12 +4476,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -4511,12 +4491,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P3890</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:ch-kyi-sherab'}</t>
         </is>
       </c>
     </row>
@@ -4526,12 +4506,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>P8277</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>{'eft:rgya-mtsho-i-sde'}</t>
+          <t>{'eft:tsultrim-gyalwa', 'eft:tshul-khrims-rgyal-ba'}</t>
         </is>
       </c>
     </row>
@@ -4541,12 +4521,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P6453</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:tsultrim-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -4556,12 +4536,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>P5788</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>{'eft:th-nmi-sambhota'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -4571,12 +4551,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -4586,12 +4566,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
incorporate existing 84000 attributes, while avoiding duplicates
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -3486,12 +3486,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:palgyi-lh-npo', 'eft:dpal-gyi-lhun-po', 'eft:ban-de-dpal-gyi-lhun-po'}</t>
         </is>
       </c>
     </row>
@@ -3501,12 +3501,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -3516,12 +3516,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P8212</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:devendraraksita'}</t>
         </is>
       </c>
     </row>
@@ -3531,12 +3531,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -3546,12 +3546,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:bidyakaraprabha', 'eft:vidyakaraprabha'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -3561,12 +3561,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P1242</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:g-wai-lodr-'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -3576,12 +3576,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-dpal', 'eft:gew-pal'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -3591,12 +3591,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -3606,12 +3606,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P8221</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:g-ch-drup'}</t>
+          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
         </is>
       </c>
     </row>
@@ -3621,12 +3621,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P1242</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po', 'eft:palgyi-lh-npo'}</t>
+          <t>{'eft:g-wai-lodr-'}</t>
         </is>
       </c>
     </row>
@@ -3636,12 +3636,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P2551</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:blo-ldan-shes-rab'}</t>
         </is>
       </c>
     </row>
@@ -3651,12 +3651,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:cog-ro-klu-i-rgyal-mtshan', 'eft:klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:bidyakaraprabha', 'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -3666,12 +3666,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -3681,12 +3681,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3696,12 +3696,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P2557</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:-brom-rgyal-ba-i-byung-gnas', 'eft:-brom'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3711,12 +3711,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:ch-nyi-tsultrim', 'eft:lotsawa-band-dharmatasila', 'eft:dharmatasila'}</t>
         </is>
       </c>
     </row>
@@ -3726,12 +3726,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P3458</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:g-lhets-'}</t>
         </is>
       </c>
     </row>
@@ -3741,12 +3741,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P8276</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'eft:wang-phab-zhwun-wang-phan-zhun-'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -3756,12 +3756,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:band-paltsek', 'eft:paltsek', 'eft:ska-ba-dpal-brtsegs', 'eft:ban-de-dpal-brtsegs', 'eft:dpal-brtsegs'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -3771,12 +3771,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P8280</t>
+          <t>P8221</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:subhasita'}</t>
+          <t>{'eft:g-ch-drup'}</t>
         </is>
       </c>
     </row>
@@ -3786,12 +3786,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P5788</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:th-nmi-sambhota'}</t>
         </is>
       </c>
     </row>
@@ -3801,12 +3801,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:ch-nyi-tsultrim', 'eft:lotsawa-band-dharmatasila', 'eft:dharmatasila'}</t>
+          <t>{'eft:dipamkara-srijnana', 'eft:dipamkarasrijnana'}</t>
         </is>
       </c>
     </row>
@@ -3816,12 +3816,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P2614</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:nyen-lotsawa-darma-drak'}</t>
         </is>
       </c>
     </row>
@@ -3831,12 +3831,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P3890</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:ch-kyi-sherab'}</t>
         </is>
       </c>
     </row>
@@ -3846,12 +3846,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
     </row>
@@ -3861,12 +3861,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:yesh-nyingpo', 'eft:ye-shes-snying-po', 'eft:t-jnanagarbha'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -3876,12 +3876,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzag-po', 'eft:rinchen-zangpo', 'eft:rin-chen-bzang-po'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -3891,12 +3891,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P4CZ15308</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
+          <t>{'eft:vairocanaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3906,12 +3906,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P3458</t>
+          <t>P8278</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:g-lhets-'}</t>
+          <t>{'eft:gewai-lodr-', 'eft:dge-ba-i-blo-gros'}</t>
         </is>
       </c>
     </row>
@@ -3921,12 +3921,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:jinamitra-k-', 'eft:jinamitra', 'eft:dzi-na-mi-tra-k-'}</t>
         </is>
       </c>
     </row>
@@ -3936,12 +3936,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -3951,12 +3951,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags', 'eft:patsap-nyima-drak-'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -3966,12 +3966,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -3981,12 +3981,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P8216</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:sakya-lodr-'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -3996,12 +3996,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P8276</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:wang-phab-zhwun-wang-phan-zhun-'}</t>
         </is>
       </c>
     </row>
@@ -4011,12 +4011,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -4026,12 +4026,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P8277</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
+          <t>{'eft:rgya-mtsho-i-sde'}</t>
         </is>
       </c>
     </row>
@@ -4041,12 +4041,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P2614</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:nyen-lotsawa-darma-drak'}</t>
+          <t>{'eft:zhang-yesh-d-', 'eft:band-yesh-d-', 'eft:yesh-de', 'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:band-yesh-de', 'eft:yesh-d-ye-shes-sde-'}</t>
         </is>
       </c>
     </row>
@@ -4056,12 +4056,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P4CZ15308</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:vairocanaraksita'}</t>
+          <t>{'eft:rin-chen-bzag-po', 'eft:rinchen-zangpo', 'eft:rin-chen-bzang-po'}</t>
         </is>
       </c>
     </row>
@@ -4071,12 +4071,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P8278</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:gewai-lodr-', 'eft:dge-ba-i-blo-gros'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba', 'eft:tsultrim-gyalwa'}</t>
         </is>
       </c>
     </row>
@@ -4086,12 +4086,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
         </is>
       </c>
     </row>
@@ -4101,12 +4101,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P4256</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:lotsawa-zangkyong-bzang-skyong-'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -4121,7 +4121,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:vajrvisramitra', 'eft:sherap-', 'eft:sakyasena'}</t>
+          <t>{'eft:sherap-', 'eft:sakyasena', 'eft:vajrvisramitra'}</t>
         </is>
       </c>
     </row>
@@ -4131,12 +4131,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P4256</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:lotsawa-zangkyong-bzang-skyong-'}</t>
         </is>
       </c>
     </row>
@@ -4146,12 +4146,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:silendrabodhi', 'eft:surendrabodhi', 'eft:srilendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -4161,12 +4161,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P8212</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:devendraraksita'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -4176,12 +4176,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P8271</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:kumararaksita'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -4191,12 +4191,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:patsap-nyima-drak-', 'eft:pa-tshab-nyi-ma-grags'}</t>
         </is>
       </c>
     </row>
@@ -4206,12 +4206,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -4221,12 +4221,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P8271</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:kumararaksita'}</t>
         </is>
       </c>
     </row>
@@ -4236,12 +4236,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:band-yesh-d-', 'eft:yesh-de', 'eft:yesh-d-', 'eft:zhang-yesh-d-', 'eft:band-yesh-de', 'eft:ye-shes-sde', 'eft:yesh-d-ye-shes-sde-'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -4251,12 +4251,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:srilendrabodhi', 'eft:surendrabodhi', 'eft:silendrabodhi'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -4266,12 +4266,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P8280</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:subhasita'}</t>
         </is>
       </c>
     </row>
@@ -4281,12 +4281,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P8216</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:sakya-lodr-'}</t>
         </is>
       </c>
     </row>
@@ -4296,12 +4296,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>P2551</t>
+          <t>P8249</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>{'eft:blo-ldan-shes-rab'}</t>
+          <t>{'eft:pandita-dharmakara', 'eft:dharmakara'}</t>
         </is>
       </c>
     </row>
@@ -4311,12 +4311,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:rinchen-tso', 'eft:rin-chen-tsho'}</t>
         </is>
       </c>
     </row>
@@ -4326,12 +4326,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>P5788</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>{'eft:th-nmi-sambhota'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:ye-shes-snying-po', 'eft:yesh-nyingpo'}</t>
         </is>
       </c>
     </row>
@@ -4341,12 +4341,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P6453</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:tsultrim-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -4356,12 +4356,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>P8249</t>
+          <t>P2557</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>{'eft:pandita-dharmakara', 'eft:dharmakara'}</t>
+          <t>{'eft:-brom', 'eft:-brom-rgyal-ba-i-byung-gnas'}</t>
         </is>
       </c>
     </row>
@@ -4371,12 +4371,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -4386,12 +4386,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:dzi-na-mi-tra-k-', 'eft:jinamitra-k-'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -4401,12 +4401,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>P1321</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>{'eft:shang-buchikpa'}</t>
+          <t>{'eft:prajnavarma', 'eft:prajnavarman'}</t>
         </is>
       </c>
     </row>
@@ -4416,12 +4416,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -4431,12 +4431,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
+          <t>{'eft:ban-de-dpal-brtsegs', 'eft:ska-ba-dpal-brtsegs', 'eft:band-paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:paltsek'}</t>
         </is>
       </c>
     </row>
@@ -4446,12 +4446,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -4461,12 +4461,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>P8277</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>{'eft:rgya-mtsho-i-sde'}</t>
+          <t>{'eft:gew-pal', 'eft:dge-ba-dpal'}</t>
         </is>
       </c>
     </row>
@@ -4476,12 +4476,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -4491,12 +4491,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>P3890</t>
+          <t>P1321</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>{'eft:ch-kyi-sherab'}</t>
+          <t>{'eft:shang-buchikpa'}</t>
         </is>
       </c>
     </row>
@@ -4506,12 +4506,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>{'eft:tsultrim-gyalwa', 'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -4521,12 +4521,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>P6453</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>{'eft:tsultrim-gyaltsen'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -4536,12 +4536,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -4551,12 +4551,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -4566,12 +4566,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
load files with relative paths
</commit_message>
<xml_diff>
--- a/all_person_matches.xlsx
+++ b/all_person_matches.xlsx
@@ -3486,12 +3486,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>P8093</t>
+          <t>P2614</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'eft:kamalagupta'}</t>
+          <t>{'eft:nyen-lotsawa-darma-drak'}</t>
         </is>
       </c>
     </row>
@@ -3501,12 +3501,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P8182</t>
+          <t>P8261</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'eft:paltsek', 'eft:ban-de-dpal-brtsegs', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:dpal-brtsegs', 'eft:band-paltsek', 'eft:ska-ba-dpal-brtsegs'}</t>
+          <t>{'eft:munivarman', 'eft:munivarma'}</t>
         </is>
       </c>
     </row>
@@ -3516,12 +3516,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>P3709</t>
+          <t>P00KG07267</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'eft:phakpa-sherab'}</t>
+          <t>{'eft:sarvajnadeva', 'eft:sarvanyadeva'}</t>
         </is>
       </c>
     </row>
@@ -3531,12 +3531,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>P8245</t>
+          <t>P2551</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'eft:buddhakaravarma'}</t>
+          <t>{'eft:blo-ldan-shes-rab'}</t>
         </is>
       </c>
     </row>
@@ -3546,12 +3546,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>P8205</t>
+          <t>P8273</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'eft:yesh-d-', 'eft:ye-shes-sde', 'eft:zhang-yesh-d-', 'eft:yesh-de', 'eft:yesh-d-ye-shes-sde-', 'eft:band-yesh-de', 'eft:band-yesh-d-'}</t>
+          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
         </is>
       </c>
     </row>
@@ -3561,12 +3561,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>P8213</t>
+          <t>P5788</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
+          <t>{'eft:th-nmi-sambhota'}</t>
         </is>
       </c>
     </row>
@@ -3576,12 +3576,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>P3890</t>
+          <t>P8213</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'eft:ch-kyi-sherab'}</t>
+          <t>{'eft:t-vidyakarasimha', 'eft:vidyakarasimha'}</t>
         </is>
       </c>
     </row>
@@ -3591,12 +3591,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>P8278</t>
+          <t>P2548</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'eft:dge-ba-i-blo-gros', 'eft:gewai-lodr-'}</t>
+          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
         </is>
       </c>
     </row>
@@ -3606,12 +3606,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>P8260</t>
+          <t>P8222</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'eft:dpal-dbyangs'}</t>
+          <t>{'eft:jnanasidhi', 'eft:jnanasiddhi'}</t>
         </is>
       </c>
     </row>
@@ -3621,12 +3621,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>P5788</t>
+          <t>P8268</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'eft:th-nmi-sambhota'}</t>
+          <t>{'eft:buddhaprabha'}</t>
         </is>
       </c>
     </row>
@@ -3636,12 +3636,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>P8216</t>
+          <t>P8182</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'eft:sakya-lodr-'}</t>
+          <t>{'eft:band-paltsek', 'eft:kawa-paltsek-under-the-name-paltsek-raksita-', 'eft:ska-ba-dpal-brtsegs', 'eft:dpal-brtsegs', 'eft:paltsek', 'eft:ban-de-dpal-brtsegs'}</t>
         </is>
       </c>
     </row>
@@ -3651,12 +3651,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>P8273</t>
+          <t>P3709</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-tsho', 'eft:rinchen-tso'}</t>
+          <t>{'eft:phakpa-sherab'}</t>
         </is>
       </c>
     </row>
@@ -3666,12 +3666,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>P8271</t>
+          <t>P3214</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'eft:kumararaksita'}</t>
+          <t>{'eft:danasila'}</t>
         </is>
       </c>
     </row>
@@ -3681,12 +3681,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>P1242</t>
+          <t>P4263</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'eft:g-wai-lodr-'}</t>
+          <t>{'eft:dge-ba-dpal', 'eft:gew-pal'}</t>
         </is>
       </c>
     </row>
@@ -3696,12 +3696,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>P8228</t>
+          <t>P3456</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'eft:surendrabodhi'}</t>
+          <t>{'eft:tshul-khrims-rgyal-ba', 'eft:tsultrim-gyalwa'}</t>
         </is>
       </c>
     </row>
@@ -3711,12 +3711,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>P4255</t>
+          <t>P8217</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:ye-shes-snying-po', 'eft:yesh-nyingpo'}</t>
+          <t>{'eft:jnanagarbha', 'eft:t-jnanagarbha'}</t>
         </is>
       </c>
     </row>
@@ -3726,12 +3726,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>P4256</t>
+          <t>P8220</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'eft:lotsawa-zangkyong-bzang-skyong-'}</t>
+          <t>{'eft:devacandra'}</t>
         </is>
       </c>
     </row>
@@ -3756,12 +3756,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P8171</t>
+          <t>P0TMP092</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'eft:dharmasribhadra'}</t>
+          <t>{'eft:anandasri-s-'}</t>
         </is>
       </c>
     </row>
@@ -3771,12 +3771,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P4242</t>
+          <t>P8271</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'eft:sherab-lekpa'}</t>
+          <t>{'eft:kumararaksita'}</t>
         </is>
       </c>
     </row>
@@ -3786,12 +3786,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P4258</t>
+          <t>P0TMPT007</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'eft:dpal-byor'}</t>
+          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
         </is>
       </c>
     </row>
@@ -3801,12 +3801,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P3285</t>
+          <t>P4259</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'eft:sakya-yesh-'}</t>
+          <t>{'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po'}</t>
         </is>
       </c>
     </row>
@@ -3816,12 +3816,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>P8263</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'eft:sakyasena', 'eft:sherap-', 'eft:vajrvisramitra'}</t>
+          <t>{'eft:leki-d-'}</t>
         </is>
       </c>
     </row>
@@ -3831,12 +3831,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P4CZ16780</t>
+          <t>P8276</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'eft:manjusrigarbha'}</t>
+          <t>{'eft:wang-phab-zhwun-wang-phan-zhun-'}</t>
         </is>
       </c>
     </row>
@@ -3846,12 +3846,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P8276</t>
+          <t>P8212</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'eft:wang-phab-zhwun-wang-phan-zhun-'}</t>
+          <t>{'eft:devendraraksita'}</t>
         </is>
       </c>
     </row>
@@ -3861,12 +3861,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P8277</t>
+          <t>P4258</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>{'eft:rgya-mtsho-i-sde'}</t>
+          <t>{'eft:dpal-byor'}</t>
         </is>
       </c>
     </row>
@@ -3876,12 +3876,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P2614</t>
+          <t>P3285</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>{'eft:nyen-lotsawa-darma-drak'}</t>
+          <t>{'eft:sakya-yesh-'}</t>
         </is>
       </c>
     </row>
@@ -3891,12 +3891,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P3458</t>
+          <t>P8265</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>{'eft:g-lhets-'}</t>
+          <t>{'eft:ratnaraksita'}</t>
         </is>
       </c>
     </row>
@@ -3906,12 +3906,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
+          <t>P0TMP080</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>{'eft:siladharma'}</t>
+          <t>{'eft:hwa-shang-zab-mo'}</t>
         </is>
       </c>
     </row>
@@ -3921,12 +3921,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P8265</t>
+          <t>P0RK8</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>{'eft:ratnaraksita'}</t>
+          <t>{'eft:dharmapala'}</t>
         </is>
       </c>
     </row>
@@ -3936,12 +3936,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P8206</t>
+          <t>P8216</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>{'eft:celu'}</t>
+          <t>{'eft:sakya-lodr-'}</t>
         </is>
       </c>
     </row>
@@ -3951,12 +3951,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P2956</t>
+          <t>P4256</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>{'eft:krsnapandita'}</t>
+          <t>{'eft:lotsawa-zangkyong-bzang-skyong-'}</t>
         </is>
       </c>
     </row>
@@ -3966,12 +3966,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P8266</t>
+          <t>P8277</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>{'eft:lotsawa-band-dharmatasila', 'eft:ch-nyi-tsultrim', 'eft:dharmatasila'}</t>
+          <t>{'eft:rgya-mtsho-i-sde'}</t>
         </is>
       </c>
     </row>
@@ -3981,12 +3981,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P0TMPT007</t>
+          <t>P2956</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>{'eft:rnam-par-mi-rtog-pa'}</t>
+          <t>{'eft:krsnapandita'}</t>
         </is>
       </c>
     </row>
@@ -3996,12 +3996,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P4CZ15137</t>
+          <t>?</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>{'eft:kumarakalasa'}</t>
+          <t>{'eft:sherap-', 'eft:sakyasena', 'eft:vajrvisramitra'}</t>
         </is>
       </c>
     </row>
@@ -4011,12 +4011,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P8268</t>
+          <t>P4CZ16819</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>{'eft:buddhaprabha'}</t>
+          <t>{'eft:sakyaprabha'}</t>
         </is>
       </c>
     </row>
@@ -4026,12 +4026,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P8222</t>
+          <t>P8245</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>{'eft:jnanasiddhi', 'eft:jnanasidhi'}</t>
+          <t>{'eft:buddhakaravarma'}</t>
         </is>
       </c>
     </row>
@@ -4041,12 +4041,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P6453</t>
+          <t>P8221</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>{'eft:tsultrim-gyaltsen'}</t>
+          <t>{'eft:g-ch-drup'}</t>
         </is>
       </c>
     </row>
@@ -4056,12 +4056,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P1KG8854</t>
+          <t>P3890</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>{'eft:silendrabodhi', 'eft:srilendrabodhi', 'eft:surendrabodhi'}</t>
+          <t>{'eft:ch-kyi-sherab'}</t>
         </is>
       </c>
     </row>
@@ -4071,12 +4071,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P3379</t>
+          <t>P2637</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
+          <t>{'eft:trakpa-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -4086,12 +4086,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P8261</t>
+          <t>P4CZ16780</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>{'eft:munivarman', 'eft:munivarma'}</t>
+          <t>{'eft:manjusrigarbha'}</t>
         </is>
       </c>
     </row>
@@ -4101,12 +4101,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P8217</t>
+          <t>P8171</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>{'eft:t-jnanagarbha', 'eft:jnanagarbha'}</t>
+          <t>{'eft:dharmasribhadra'}</t>
         </is>
       </c>
     </row>
@@ -4116,12 +4116,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P8267</t>
+          <t>P8211</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>{'eft:vijayasila'}</t>
+          <t>{'eft:bidyakaraprabha', 'eft:vidyakaraprabha'}</t>
         </is>
       </c>
     </row>
@@ -4131,12 +4131,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P753</t>
+          <t>P8260</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>{'eft:rin-chen-bzang-po', 'eft:rinchen-zangpo', 'eft:rin-chen-bzag-po'}</t>
+          <t>{'eft:dpal-dbyangs'}</t>
         </is>
       </c>
     </row>
@@ -4146,12 +4146,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P00KG07267</t>
+          <t>P4CZ15137</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>{'eft:sarvanyadeva', 'eft:sarvajnadeva'}</t>
+          <t>{'eft:kumarakalasa'}</t>
         </is>
       </c>
     </row>
@@ -4161,12 +4161,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P8263</t>
+          <t>P1KG8854</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>{'eft:leki-d-'}</t>
+          <t>{'eft:silendrabodhi', 'eft:srilendrabodhi', 'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -4176,12 +4176,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P2637</t>
+          <t>P0TMP098</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>{'eft:trakpa-gyaltsen'}</t>
+          <t>{'eft:jinavara'}</t>
         </is>
       </c>
     </row>
@@ -4191,12 +4191,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P1321</t>
+          <t>P8219</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>{'eft:shang-buchikpa'}</t>
+          <t>{'eft:visuddhasimha'}</t>
         </is>
       </c>
     </row>
@@ -4206,12 +4206,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P0TMP080</t>
+          <t>P8266</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>{'eft:hwa-shang-zab-mo'}</t>
+          <t>{'eft:lotsawa-band-dharmatasila', 'eft:dharmatasila', 'eft:ch-nyi-tsultrim'}</t>
         </is>
       </c>
     </row>
@@ -4221,12 +4221,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P2551</t>
+          <t>P8205</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>{'eft:blo-ldan-shes-rab'}</t>
+          <t>{'eft:band-yesh-de', 'eft:ye-shes-sde', 'eft:yesh-de', 'eft:zhang-yesh-d-', 'eft:band-yesh-d-', 'eft:yesh-d-ye-shes-sde-', 'eft:yesh-d-'}</t>
         </is>
       </c>
     </row>
@@ -4236,12 +4236,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P8280</t>
+          <t>P4255</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>{'eft:subhasita'}</t>
+          <t>{'eft:t-jnanagarbha', 'eft:yesh-nyingpo', 'eft:ye-shes-snying-po'}</t>
         </is>
       </c>
     </row>
@@ -4251,12 +4251,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P4263</t>
+          <t>P1321</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>{'eft:gew-pal', 'eft:dge-ba-dpal'}</t>
+          <t>{'eft:shang-buchikpa'}</t>
         </is>
       </c>
     </row>
@@ -4266,12 +4266,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P3214</t>
+          <t>P8209</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>{'eft:danasila'}</t>
+          <t>{'eft:dzi-na-mi-tra-k-', 'eft:jinamitra', 'eft:jinamitra-k-'}</t>
         </is>
       </c>
     </row>
@@ -4281,12 +4281,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P8209</t>
+          <t>P0TMP104</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>{'eft:jinamitra', 'eft:jinamitra-k-', 'eft:dzi-na-mi-tra-k-'}</t>
+          <t>{'eft:punyasambhava'}</t>
         </is>
       </c>
     </row>
@@ -4296,12 +4296,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>P8219</t>
+          <t>P8267</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>{'eft:visuddhasimha'}</t>
+          <t>{'eft:vijayasila'}</t>
         </is>
       </c>
     </row>
@@ -4311,12 +4311,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>P3456</t>
+          <t>P4CZ15308</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>{'eft:tsultrim-gyalwa', 'eft:tshul-khrims-rgyal-ba'}</t>
+          <t>{'eft:vairocanaraksita'}</t>
         </is>
       </c>
     </row>
@@ -4326,12 +4326,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>P8221</t>
+          <t>P3379</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>{'eft:g-ch-drup'}</t>
+          <t>{'eft:dipamkarasrijnana', 'eft:dipamkara-srijnana'}</t>
         </is>
       </c>
     </row>
@@ -4341,12 +4341,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>P0TMP104</t>
+          <t>P8183</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>{'eft:punyasambhava'}</t>
+          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
         </is>
       </c>
     </row>
@@ -4356,12 +4356,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>P0TMP098</t>
+          <t>P753</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>{'eft:jinavara'}</t>
+          <t>{'eft:rin-chen-bzag-po', 'eft:rin-chen-bzang-po', 'eft:rinchen-zangpo'}</t>
         </is>
       </c>
     </row>
@@ -4371,12 +4371,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>P8183</t>
+          <t>P8093</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>{'eft:klu-i-rgyal-mtshan', 'eft:cog-ro-klu-i-rgyal-mtshan'}</t>
+          <t>{'eft:kamalagupta'}</t>
         </is>
       </c>
     </row>
@@ -4386,12 +4386,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>P4CZ16819</t>
+          <t>P8206</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>{'eft:sakyaprabha'}</t>
+          <t>{'eft:celu'}</t>
         </is>
       </c>
     </row>
@@ -4401,12 +4401,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>P0RK8</t>
+          <t>P6453</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>{'eft:dharmapala'}</t>
+          <t>{'eft:tsultrim-gyaltsen'}</t>
         </is>
       </c>
     </row>
@@ -4416,12 +4416,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>P2548</t>
+          <t>https://lod.dila.edu.tw/resource.php?id=A000089</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>{'eft:prajnavarman', 'eft:prajnavarma'}</t>
+          <t>{'eft:siladharma'}</t>
         </is>
       </c>
     </row>
@@ -4431,12 +4431,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>P0TMP092</t>
+          <t>P8151</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>{'eft:anandasri-s-'}</t>
+          <t>{'eft:gayadhara'}</t>
         </is>
       </c>
     </row>
@@ -4446,12 +4446,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>P4259</t>
+          <t>P4242</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>{'eft:palgyi-lh-npo', 'eft:ban-de-dpal-gyi-lhun-po', 'eft:dpal-gyi-lhun-po'}</t>
+          <t>{'eft:sherab-lekpa'}</t>
         </is>
       </c>
     </row>
@@ -4461,12 +4461,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>P4CZ15308</t>
+          <t>P5651</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>{'eft:vairocanaraksita'}</t>
+          <t>{'eft:pa-tshab-nyi-ma-grags', 'eft:patsap-nyima-drak-'}</t>
         </is>
       </c>
     </row>
@@ -4476,12 +4476,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>P5651</t>
+          <t>P8228</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>{'eft:pa-tshab-nyi-ma-grags', 'eft:patsap-nyima-drak-'}</t>
+          <t>{'eft:surendrabodhi'}</t>
         </is>
       </c>
     </row>
@@ -4491,12 +4491,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>P8220</t>
+          <t>P8269</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>{'eft:devacandra'}</t>
+          <t>{'eft:dgon-gling-rma'}</t>
         </is>
       </c>
     </row>
@@ -4506,12 +4506,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>P8269</t>
+          <t>P8278</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>{'eft:dgon-gling-rma'}</t>
+          <t>{'eft:dge-ba-i-blo-gros', 'eft:gewai-lodr-'}</t>
         </is>
       </c>
     </row>
@@ -4521,12 +4521,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>P8212</t>
+          <t>P2557</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>{'eft:devendraraksita'}</t>
+          <t>{'eft:-brom', 'eft:-brom-rgyal-ba-i-byung-gnas'}</t>
         </is>
       </c>
     </row>
@@ -4536,12 +4536,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>P8211</t>
+          <t>P1242</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>{'eft:vidyakaraprabha', 'eft:bidyakaraprabha'}</t>
+          <t>{'eft:g-wai-lodr-'}</t>
         </is>
       </c>
     </row>
@@ -4551,12 +4551,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>P2557</t>
+          <t>P8280</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>{'eft:-brom-rgyal-ba-i-byung-gnas', 'eft:-brom'}</t>
+          <t>{'eft:subhasita'}</t>
         </is>
       </c>
     </row>
@@ -4566,12 +4566,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>P8151</t>
+          <t>P3458</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>{'eft:gayadhara'}</t>
+          <t>{'eft:g-lhets-'}</t>
         </is>
       </c>
     </row>

</xml_diff>